<commit_message>
Mise à jour du FAST et du pieuvre
</commit_message>
<xml_diff>
--- a/FAST_raffine.xlsx
+++ b/FAST_raffine.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10720" yWindow="0" windowWidth="15040" windowHeight="15240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -866,7 +866,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
-            <a:t>FP1 : Enregistrer les données nécessaire à la détection de l'individu</a:t>
+            <a:t>FP1 : Enregistrer les données nécessaire à la détection du mouvement de l'oeil</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR"/>
         </a:p>
@@ -1014,7 +1014,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
-            <a:t>FP22 : Détecter l'oeil</a:t>
+            <a:t>FP222 : Détecter l'oeil</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -1078,43 +1078,6 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{7E92DBF9-0282-3B4B-9193-15656C09A041}">
-      <dgm:prSet phldrT="[Texte]"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
-            <a:t>FP14 : Compresser les données</a:t>
-          </a:r>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{84C2140E-F94B-3A42-9984-32D5D0D67690}" type="parTrans" cxnId="{1D5BC62B-2A2D-3D4B-BFBC-1F8D84208103}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{030D0447-EF41-D64C-8E70-01DF93EB72FB}" type="sibTrans" cxnId="{1D5BC62B-2A2D-3D4B-BFBC-1F8D84208103}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
     <dgm:pt modelId="{B1871CE9-AA57-7E40-9F44-89545C773C31}">
       <dgm:prSet phldrT="[Texte]"/>
       <dgm:spPr/>
@@ -1226,43 +1189,6 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{4EFBB3C4-F314-AA40-AA6F-6D4A76AA74FE}">
-      <dgm:prSet phldrT="[Texte]"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
-            <a:t>Carte de traitement</a:t>
-          </a:r>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{518D05D7-25EC-904D-AC1F-588DEE03B23D}" type="parTrans" cxnId="{2DA17B3E-21EE-964C-969D-3D2CF2623715}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{7B51DE5B-F28F-1E43-A96A-418E2C1195DE}" type="sibTrans" cxnId="{2DA17B3E-21EE-964C-969D-3D2CF2623715}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
     <dgm:pt modelId="{CBD00C11-7705-4B46-A507-504E11D7B2C4}">
       <dgm:prSet phldrT="[Texte]"/>
       <dgm:spPr/>
@@ -1336,7 +1262,7 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{2064DC40-2F6A-7246-96EB-B7DCB07874C8}">
+    <dgm:pt modelId="{EB608E93-0479-2148-BCC1-5BA22B50A826}">
       <dgm:prSet phldrT="[Texte]"/>
       <dgm:spPr/>
       <dgm:t>
@@ -1345,12 +1271,12 @@
         <a:p>
           <a:r>
             <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
-            <a:t>FP24 : Analyser le mouvement de la pupille</a:t>
+            <a:t>FP4 : Agir sur l'IHM</a:t>
           </a:r>
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{898D5F8F-CA92-7B4D-9D96-13C7CC8EB24F}" type="parTrans" cxnId="{A467DF2D-BC30-E045-8362-C42E60148128}">
+    <dgm:pt modelId="{DE6250AC-E2C3-EA4C-90F4-F144D5C45412}" type="parTrans" cxnId="{507C37D9-DF70-C049-AB45-6D6194C6EDD1}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1361,7 +1287,7 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{DBD9B648-1F16-814B-85AA-41C3AC0F5A3F}" type="sibTrans" cxnId="{A467DF2D-BC30-E045-8362-C42E60148128}">
+    <dgm:pt modelId="{873FE768-EBDB-5444-A928-15F6A44CCEAB}" type="sibTrans" cxnId="{507C37D9-DF70-C049-AB45-6D6194C6EDD1}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1372,7 +1298,7 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{E1246F00-5110-6146-85B3-F18EAD31DE44}">
+    <dgm:pt modelId="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}">
       <dgm:prSet phldrT="[Texte]"/>
       <dgm:spPr/>
       <dgm:t>
@@ -1381,12 +1307,12 @@
         <a:p>
           <a:r>
             <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
-            <a:t>FP25 : Déduire l'action à exécuter</a:t>
+            <a:t>FP41 : Effectuer l'action</a:t>
           </a:r>
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{A3EE15A6-3F32-E047-A7C8-658B5B9A2426}" type="parTrans" cxnId="{512615FE-EEA4-3B4F-B5DE-57D9F2585BAC}">
+    <dgm:pt modelId="{8F42AAD0-AA72-224D-89F6-60847A76B1D5}" type="parTrans" cxnId="{7BDF0CB4-4494-3841-A0C2-B96746C922B8}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1397,7 +1323,7 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{12500183-1309-E045-9F84-801F4A2275FA}" type="sibTrans" cxnId="{512615FE-EEA4-3B4F-B5DE-57D9F2585BAC}">
+    <dgm:pt modelId="{C3BA1502-7EEB-0B4D-89AF-D304786068A6}" type="sibTrans" cxnId="{7BDF0CB4-4494-3841-A0C2-B96746C922B8}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1408,7 +1334,7 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{EB608E93-0479-2148-BCC1-5BA22B50A826}">
+    <dgm:pt modelId="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}">
       <dgm:prSet phldrT="[Texte]"/>
       <dgm:spPr/>
       <dgm:t>
@@ -1417,79 +1343,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
-            <a:t>FP3 : Agir sur l'IHM</a:t>
-          </a:r>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{DE6250AC-E2C3-EA4C-90F4-F144D5C45412}" type="parTrans" cxnId="{507C37D9-DF70-C049-AB45-6D6194C6EDD1}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{873FE768-EBDB-5444-A928-15F6A44CCEAB}" type="sibTrans" cxnId="{507C37D9-DF70-C049-AB45-6D6194C6EDD1}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}">
-      <dgm:prSet phldrT="[Texte]"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
-            <a:t>FP31 : Effectuer l'action</a:t>
-          </a:r>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{8F42AAD0-AA72-224D-89F6-60847A76B1D5}" type="parTrans" cxnId="{7BDF0CB4-4494-3841-A0C2-B96746C922B8}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{C3BA1502-7EEB-0B4D-89AF-D304786068A6}" type="sibTrans" cxnId="{7BDF0CB4-4494-3841-A0C2-B96746C922B8}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}">
-      <dgm:prSet phldrT="[Texte]"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
-            <a:t>FP31 : Rendre l'action visible sur l'interface</a:t>
+            <a:t>FP42 : Rendre l'action visible sur l'interface</a:t>
           </a:r>
         </a:p>
       </dgm:t>
@@ -1697,7 +1551,43 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{94300211-45FB-9547-B995-E1E57425CDE7}">
+    <dgm:pt modelId="{C762D9DC-C267-9446-B1CC-A95E3114C015}">
+      <dgm:prSet phldrT="[Texte]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR"/>
+            <a:t>FP22 : Détecter l'individu et ses mouvements</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{B5D4559E-723E-D842-BB45-358E2F203970}" type="parTrans" cxnId="{935CFD64-B563-C14A-8843-98A8FBBCCE52}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{DA64E6F3-5664-5A48-B5C2-B7239FD965F9}" type="sibTrans" cxnId="{935CFD64-B563-C14A-8843-98A8FBBCCE52}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{DA4300B2-2331-2046-ABC1-100C122A715A}">
       <dgm:prSet phldrT="[Texte]"/>
       <dgm:spPr/>
       <dgm:t>
@@ -1706,12 +1596,12 @@
         <a:p>
           <a:r>
             <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
-            <a:t>Logiciel d'algorithmique</a:t>
+            <a:t>FP221 : Détecter l'individu</a:t>
           </a:r>
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{4FDA31E9-0995-E646-B247-48C734F29F55}" type="parTrans" cxnId="{1F843B3F-7DC5-414A-9B4E-30DCB65002A0}">
+    <dgm:pt modelId="{41576158-B990-5740-AFD7-A7F30A9E11F8}" type="parTrans" cxnId="{FB0EE346-51CC-5E4E-B766-63DAD646615F}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1722,7 +1612,7 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{CCCEAC01-3AAB-0740-B4DD-8DC6B0962AE7}" type="sibTrans" cxnId="{1F843B3F-7DC5-414A-9B4E-30DCB65002A0}">
+    <dgm:pt modelId="{ADB60117-51CE-ED4A-B44F-4D726CCCA9F0}" type="sibTrans" cxnId="{FB0EE346-51CC-5E4E-B766-63DAD646615F}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1733,7 +1623,7 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{1FCD6FA2-2EC1-E044-8817-90704567D52F}">
+    <dgm:pt modelId="{0B970462-F13C-4D48-A4B7-10C043EEEE2B}">
       <dgm:prSet phldrT="[Texte]"/>
       <dgm:spPr/>
       <dgm:t>
@@ -1742,12 +1632,12 @@
         <a:p>
           <a:r>
             <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
-            <a:t>Logiciel d'algorithmique</a:t>
+            <a:t>FP223 : Détecter la pupille</a:t>
           </a:r>
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{98BE4178-0B33-D54A-91F1-7CD2B3AC77E2}" type="parTrans" cxnId="{DD6FAD2D-F789-6F4A-B4A8-DF09C8211A34}">
+    <dgm:pt modelId="{BE5B9591-AC80-4946-8C78-D7570297C39E}" type="parTrans" cxnId="{87500F0C-3129-4043-A941-9960C7FDFE5F}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1758,7 +1648,187 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{AB2C0215-39C8-5D44-ABC6-4F4701B566BF}" type="sibTrans" cxnId="{DD6FAD2D-F789-6F4A-B4A8-DF09C8211A34}">
+    <dgm:pt modelId="{9C7B62F8-4A99-4948-9007-9C010A739C17}" type="sibTrans" cxnId="{87500F0C-3129-4043-A941-9960C7FDFE5F}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{3E620EDA-5ADD-CC44-8C95-9FC1DF254361}">
+      <dgm:prSet phldrT="[Texte]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
+            <a:t>FP224 : Détecter le mouvement de la pupille</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{2E18F920-A737-724D-B818-02F6FE67E8FC}" type="parTrans" cxnId="{F081B073-88FE-7A4B-ACC7-EF443E1B1B14}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{20F03020-DD6C-8D40-A3F0-3669680E55C0}" type="sibTrans" cxnId="{F081B073-88FE-7A4B-ACC7-EF443E1B1B14}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{30615BCE-5A85-DD4B-B246-1B251E40150B}">
+      <dgm:prSet phldrT="[Texte]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
+            <a:t>FP225 : Détecter le clignement de l'oeil</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{E2540CE2-F2F8-7D4E-8EF4-139718573F86}" type="parTrans" cxnId="{E5A2EB47-D342-B941-A52E-C9F38CB342A7}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{A7ADF9D2-AE55-6249-BF7E-757C29AF0CBB}" type="sibTrans" cxnId="{E5A2EB47-D342-B941-A52E-C9F38CB342A7}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{652DE9CE-379E-5542-8267-C153E850CFF5}">
+      <dgm:prSet phldrT="[Texte]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
+            <a:t>FP3 : Interpréter les données pour déduire l'action à exécuter</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{FA9F03C1-DE3A-9849-9BB9-A7264514AC98}" type="parTrans" cxnId="{35E19FD6-62B7-8F49-8A6C-46141C8170F3}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{CC539F88-89BB-FB4D-9B01-F4D04CA5A22B}" type="sibTrans" cxnId="{35E19FD6-62B7-8F49-8A6C-46141C8170F3}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{6DC6F20A-841D-E944-B9FD-E1D140F60C2C}">
+      <dgm:prSet phldrT="[Texte]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
+            <a:t>FP31 : Analyser le mouvement de la pupille à l'aide de la distance utilisateur-IHM</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{F97D5CCC-FB1C-BD4D-8FC0-8444F262955E}" type="parTrans" cxnId="{A0B591C8-1181-A84C-AA49-A19911497FC6}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{20099B97-FDBD-6248-9B06-7F3AE556C86C}" type="sibTrans" cxnId="{A0B591C8-1181-A84C-AA49-A19911497FC6}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{5E402F45-6CF9-7D49-9393-47131AFD7CE6}">
+      <dgm:prSet phldrT="[Texte]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" b="0" i="0" u="none"/>
+            <a:t>FP32 : Déduire l'action à effectuer</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{551B3FB5-3F7C-9046-B05E-7E0316CCFFDC}" type="parTrans" cxnId="{32F68E96-4401-3C41-932F-35D7D240B538}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{9798B304-7A19-9E4B-9BF5-6944B6DC86F3}" type="sibTrans" cxnId="{32F68E96-4401-3C41-932F-35D7D240B538}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1780,6 +1850,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{C892B71B-46E3-4844-994D-39FDFFD52BCE}" type="pres">
       <dgm:prSet presAssocID="{3D5AE65B-9194-A04D-98AC-695DC8D2BA16}" presName="root1" presStyleCnt="0"/>
@@ -1805,19 +1882,33 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{1AEC4C7F-8B5D-9C4A-A0BA-DF9BE251EB21}" type="pres">
-      <dgm:prSet presAssocID="{66816B50-209E-8A44-99FF-FCA0FE6010CF}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="3"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{66816B50-209E-8A44-99FF-FCA0FE6010CF}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="4"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{2680328F-7469-384B-A713-47DAA1730724}" type="pres">
-      <dgm:prSet presAssocID="{66816B50-209E-8A44-99FF-FCA0FE6010CF}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="3"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{66816B50-209E-8A44-99FF-FCA0FE6010CF}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="4"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{A3B1B5D7-C566-0E41-9746-D2F43EE353EB}" type="pres">
       <dgm:prSet presAssocID="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" presName="root2" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{02E0FECA-2589-C94E-8421-1373276E6CD0}" type="pres">
-      <dgm:prSet presAssocID="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="0" presStyleCnt="3">
+      <dgm:prSet presAssocID="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="0" presStyleCnt="4">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1836,19 +1927,33 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{97838F66-388F-334E-8C48-6883CD119D60}" type="pres">
-      <dgm:prSet presAssocID="{300BDE9E-F0C8-E145-A198-C90D0EF8BD49}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{300BDE9E-F0C8-E145-A198-C90D0EF8BD49}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{6089D488-F8D0-3F43-80B5-219C7DCFB589}" type="pres">
-      <dgm:prSet presAssocID="{300BDE9E-F0C8-E145-A198-C90D0EF8BD49}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{300BDE9E-F0C8-E145-A198-C90D0EF8BD49}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{9352132E-E75C-084D-BC9D-398459D59092}" type="pres">
       <dgm:prSet presAssocID="{36BBC7EB-D363-3B48-8496-AA60D47185CD}" presName="root2" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{E51D9155-7752-9D41-957A-949CC75EB761}" type="pres">
-      <dgm:prSet presAssocID="{36BBC7EB-D363-3B48-8496-AA60D47185CD}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="11">
+      <dgm:prSet presAssocID="{36BBC7EB-D363-3B48-8496-AA60D47185CD}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1867,19 +1972,33 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{9F3C9693-87FA-7F45-B58A-F884460F249C}" type="pres">
-      <dgm:prSet presAssocID="{3F5EFC20-7888-8B4C-A3B9-D9A3746FD5D9}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="0" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{3F5EFC20-7888-8B4C-A3B9-D9A3746FD5D9}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="0" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{61A4E688-2EE9-2949-9B58-3693E86C97FB}" type="pres">
-      <dgm:prSet presAssocID="{3F5EFC20-7888-8B4C-A3B9-D9A3746FD5D9}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="0" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{3F5EFC20-7888-8B4C-A3B9-D9A3746FD5D9}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="0" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{A3B8A01B-4C16-9C45-8CA0-ADD1C4EAC45E}" type="pres">
       <dgm:prSet presAssocID="{B1871CE9-AA57-7E40-9F44-89545C773C31}" presName="root2" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{09A02069-0039-4049-80CB-8B6C97B26549}" type="pres">
-      <dgm:prSet presAssocID="{B1871CE9-AA57-7E40-9F44-89545C773C31}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="0" presStyleCnt="11">
+      <dgm:prSet presAssocID="{B1871CE9-AA57-7E40-9F44-89545C773C31}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="0" presStyleCnt="13">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1898,19 +2017,33 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{6880828A-3410-E644-A3C4-2294177CC41C}" type="pres">
-      <dgm:prSet presAssocID="{DC9CCC13-49B8-F64C-B46E-A357D3F309D5}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{DC9CCC13-49B8-F64C-B46E-A357D3F309D5}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{DC59D9E9-9066-744D-ABF3-DD21BDB11BAD}" type="pres">
-      <dgm:prSet presAssocID="{DC9CCC13-49B8-F64C-B46E-A357D3F309D5}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{DC9CCC13-49B8-F64C-B46E-A357D3F309D5}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{D5F962C6-3205-2145-86EF-FD40C24806EA}" type="pres">
       <dgm:prSet presAssocID="{30FE5FD2-03E7-C142-AA91-76709434DD90}" presName="root2" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{22159CD9-4EC1-E544-98E6-9AD9F99F03AF}" type="pres">
-      <dgm:prSet presAssocID="{30FE5FD2-03E7-C142-AA91-76709434DD90}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="11">
+      <dgm:prSet presAssocID="{30FE5FD2-03E7-C142-AA91-76709434DD90}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1929,19 +2062,33 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{CB5AFF4C-0CEC-F643-96B6-DAC4ED874BEC}" type="pres">
-      <dgm:prSet presAssocID="{14BF84F4-E713-F349-BD2A-D68DD017694A}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="1" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{14BF84F4-E713-F349-BD2A-D68DD017694A}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="1" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{BCF273FF-CB93-044A-911C-F34C18ABCD3F}" type="pres">
-      <dgm:prSet presAssocID="{14BF84F4-E713-F349-BD2A-D68DD017694A}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="1" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{14BF84F4-E713-F349-BD2A-D68DD017694A}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="1" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{56D840A9-821E-5D4B-8871-CCAB60349927}" type="pres">
       <dgm:prSet presAssocID="{F7A43531-C46D-B547-B844-4520542846DA}" presName="root2" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{5A6C940B-8E0D-2541-B4EE-37D9893DC81C}" type="pres">
-      <dgm:prSet presAssocID="{F7A43531-C46D-B547-B844-4520542846DA}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="1" presStyleCnt="11">
+      <dgm:prSet presAssocID="{F7A43531-C46D-B547-B844-4520542846DA}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="1" presStyleCnt="13">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1960,19 +2107,33 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{E51D49A7-6AFC-F04F-9B53-612EDC5C173D}" type="pres">
-      <dgm:prSet presAssocID="{63E4C9E5-BCE9-274B-B154-D1722539B787}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{63E4C9E5-BCE9-274B-B154-D1722539B787}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{EC1947AE-4E19-6545-8360-1E46FEF87CE8}" type="pres">
-      <dgm:prSet presAssocID="{63E4C9E5-BCE9-274B-B154-D1722539B787}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{63E4C9E5-BCE9-274B-B154-D1722539B787}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{5CBB7974-8641-7146-9A42-C507F7DDC471}" type="pres">
       <dgm:prSet presAssocID="{8F5969EE-F8BE-0348-8A1D-523AF7ADC449}" presName="root2" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{ED82EB34-8097-994C-90F2-D4621919418A}" type="pres">
-      <dgm:prSet presAssocID="{8F5969EE-F8BE-0348-8A1D-523AF7ADC449}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="11">
+      <dgm:prSet presAssocID="{8F5969EE-F8BE-0348-8A1D-523AF7ADC449}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1991,19 +2152,33 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{7FC46335-8ED1-2E49-A7BE-E54D41297FCD}" type="pres">
-      <dgm:prSet presAssocID="{0749699B-B7C4-6140-B4CB-8D60FBCE1ECB}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="2" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{0749699B-B7C4-6140-B4CB-8D60FBCE1ECB}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="2" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{36C0C19B-3F9B-2049-BB73-D3B74079B1BA}" type="pres">
-      <dgm:prSet presAssocID="{0749699B-B7C4-6140-B4CB-8D60FBCE1ECB}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="2" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{0749699B-B7C4-6140-B4CB-8D60FBCE1ECB}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="2" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{C5780C21-D1DD-A745-8AA9-1E4DA9C5756E}" type="pres">
       <dgm:prSet presAssocID="{2F71905B-FED7-7946-BB13-3426F23C1911}" presName="root2" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{743C9E64-CA35-3346-BD28-35C33D90F652}" type="pres">
-      <dgm:prSet presAssocID="{2F71905B-FED7-7946-BB13-3426F23C1911}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="2" presStyleCnt="11">
+      <dgm:prSet presAssocID="{2F71905B-FED7-7946-BB13-3426F23C1911}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="2" presStyleCnt="13">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2021,20 +2196,34 @@
       <dgm:prSet presAssocID="{2F71905B-FED7-7946-BB13-3426F23C1911}" presName="level3hierChild" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{EAE6DA3D-6DCE-8B43-86D6-453237F6F64F}" type="pres">
-      <dgm:prSet presAssocID="{84C2140E-F94B-3A42-9984-32D5D0D67690}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{AD7BBE0F-FABE-714F-B19E-9F525577B2B5}" type="pres">
-      <dgm:prSet presAssocID="{84C2140E-F94B-3A42-9984-32D5D0D67690}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{F5455EA7-4F95-6E44-B4DD-7E31D6C976CF}" type="pres">
-      <dgm:prSet presAssocID="{7E92DBF9-0282-3B4B-9193-15656C09A041}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{AFB00BA5-37D3-4D49-ABEF-E265A327F349}" type="pres">
-      <dgm:prSet presAssocID="{7E92DBF9-0282-3B4B-9193-15656C09A041}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="11">
+    <dgm:pt modelId="{9214EDCC-7637-FA4F-A663-9416C90A1781}" type="pres">
+      <dgm:prSet presAssocID="{BC4BC998-E1F0-5B45-A719-663711F9FB23}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="4"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{884F4C54-6432-7B49-A9D9-4EA1E6971C11}" type="pres">
+      <dgm:prSet presAssocID="{BC4BC998-E1F0-5B45-A719-663711F9FB23}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="4"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{B996FCDD-2B3D-5E4F-BE3F-3B9749B49997}" type="pres">
+      <dgm:prSet presAssocID="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B895C344-133F-4340-80A0-685E27E999D6}" type="pres">
+      <dgm:prSet presAssocID="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="1" presStyleCnt="4">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2048,24 +2237,38 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{BE95D251-3395-B24E-8B8F-DEEE14D3DB84}" type="pres">
-      <dgm:prSet presAssocID="{7E92DBF9-0282-3B4B-9193-15656C09A041}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{DA2BBBC5-96AE-D245-B903-7F481B166D03}" type="pres">
-      <dgm:prSet presAssocID="{518D05D7-25EC-904D-AC1F-588DEE03B23D}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="3" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{CC83B46B-5011-A34F-BF53-6A906E35A6D8}" type="pres">
-      <dgm:prSet presAssocID="{518D05D7-25EC-904D-AC1F-588DEE03B23D}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="3" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{41391B8F-AC13-DF4C-97EE-0D164D665333}" type="pres">
-      <dgm:prSet presAssocID="{4EFBB3C4-F314-AA40-AA6F-6D4A76AA74FE}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{64CE6CC6-6955-1F47-A64D-5C4536E66E8E}" type="pres">
-      <dgm:prSet presAssocID="{4EFBB3C4-F314-AA40-AA6F-6D4A76AA74FE}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="3" presStyleCnt="11">
+    <dgm:pt modelId="{598F85C8-C84D-C143-8558-EE261698AAD1}" type="pres">
+      <dgm:prSet presAssocID="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F07A7E6F-36EA-9743-8C2B-402848A63CFF}" type="pres">
+      <dgm:prSet presAssocID="{6ECFB139-B56B-7E4E-BF1F-7CC77B2204F1}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{B0B31E67-0F2F-244A-B75D-8DB3A26F446A}" type="pres">
+      <dgm:prSet presAssocID="{6ECFB139-B56B-7E4E-BF1F-7CC77B2204F1}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{416883AF-12A5-DA49-8928-A8DAA3016112}" type="pres">
+      <dgm:prSet presAssocID="{CBD00C11-7705-4B46-A507-504E11D7B2C4}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{D0686948-65B5-CE4B-99C1-9EB45F62AC5F}" type="pres">
+      <dgm:prSet presAssocID="{CBD00C11-7705-4B46-A507-504E11D7B2C4}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2079,24 +2282,38 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{54B0ACB6-DE3A-0945-B9E2-CC9D398D1FC9}" type="pres">
-      <dgm:prSet presAssocID="{4EFBB3C4-F314-AA40-AA6F-6D4A76AA74FE}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{9214EDCC-7637-FA4F-A663-9416C90A1781}" type="pres">
-      <dgm:prSet presAssocID="{BC4BC998-E1F0-5B45-A719-663711F9FB23}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="3"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{884F4C54-6432-7B49-A9D9-4EA1E6971C11}" type="pres">
-      <dgm:prSet presAssocID="{BC4BC998-E1F0-5B45-A719-663711F9FB23}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="3"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{B996FCDD-2B3D-5E4F-BE3F-3B9749B49997}" type="pres">
-      <dgm:prSet presAssocID="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{B895C344-133F-4340-80A0-685E27E999D6}" type="pres">
-      <dgm:prSet presAssocID="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="1" presStyleCnt="3">
+    <dgm:pt modelId="{7B01EE8E-0002-8644-B406-145BE45E0878}" type="pres">
+      <dgm:prSet presAssocID="{CBD00C11-7705-4B46-A507-504E11D7B2C4}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{0458EB9C-8D95-A54A-BBFE-4EB0E4F471AD}" type="pres">
+      <dgm:prSet presAssocID="{D98F1744-A7D7-C14A-B6A1-DD15D46D8107}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="3" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{2060447F-F68C-B74F-BF84-BB6A544B165A}" type="pres">
+      <dgm:prSet presAssocID="{D98F1744-A7D7-C14A-B6A1-DD15D46D8107}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="3" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{3B569781-F5BD-5E40-B302-18DD6386FFFB}" type="pres">
+      <dgm:prSet presAssocID="{05B6BD45-2167-C941-A792-94ACB32DB4EC}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{3E1A4BA4-A92F-724C-AE87-430A70601B53}" type="pres">
+      <dgm:prSet presAssocID="{05B6BD45-2167-C941-A792-94ACB32DB4EC}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="3" presStyleCnt="13">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2110,24 +2327,24 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{598F85C8-C84D-C143-8558-EE261698AAD1}" type="pres">
-      <dgm:prSet presAssocID="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{F07A7E6F-36EA-9743-8C2B-402848A63CFF}" type="pres">
-      <dgm:prSet presAssocID="{6ECFB139-B56B-7E4E-BF1F-7CC77B2204F1}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{B0B31E67-0F2F-244A-B75D-8DB3A26F446A}" type="pres">
-      <dgm:prSet presAssocID="{6ECFB139-B56B-7E4E-BF1F-7CC77B2204F1}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{416883AF-12A5-DA49-8928-A8DAA3016112}" type="pres">
-      <dgm:prSet presAssocID="{CBD00C11-7705-4B46-A507-504E11D7B2C4}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{D0686948-65B5-CE4B-99C1-9EB45F62AC5F}" type="pres">
-      <dgm:prSet presAssocID="{CBD00C11-7705-4B46-A507-504E11D7B2C4}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="11">
+    <dgm:pt modelId="{0FCCF158-7203-874A-BC78-6D0864195E77}" type="pres">
+      <dgm:prSet presAssocID="{05B6BD45-2167-C941-A792-94ACB32DB4EC}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{36D788C9-8DB5-D74D-BDE6-649BA5A5D5B8}" type="pres">
+      <dgm:prSet presAssocID="{B5D4559E-723E-D842-BB45-358E2F203970}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="10"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{D4F4059E-9072-DD44-9070-1FDB3E4A368D}" type="pres">
+      <dgm:prSet presAssocID="{B5D4559E-723E-D842-BB45-358E2F203970}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="10"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C1382441-915F-C04A-9929-FBEA1CF2BD36}" type="pres">
+      <dgm:prSet presAssocID="{C762D9DC-C267-9446-B1CC-A95E3114C015}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C6AA8951-971D-8D46-A6B7-A3287247CC64}" type="pres">
+      <dgm:prSet presAssocID="{C762D9DC-C267-9446-B1CC-A95E3114C015}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2141,24 +2358,24 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{7B01EE8E-0002-8644-B406-145BE45E0878}" type="pres">
-      <dgm:prSet presAssocID="{CBD00C11-7705-4B46-A507-504E11D7B2C4}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{0458EB9C-8D95-A54A-BBFE-4EB0E4F471AD}" type="pres">
-      <dgm:prSet presAssocID="{D98F1744-A7D7-C14A-B6A1-DD15D46D8107}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="4" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{2060447F-F68C-B74F-BF84-BB6A544B165A}" type="pres">
-      <dgm:prSet presAssocID="{D98F1744-A7D7-C14A-B6A1-DD15D46D8107}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="4" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{3B569781-F5BD-5E40-B302-18DD6386FFFB}" type="pres">
-      <dgm:prSet presAssocID="{05B6BD45-2167-C941-A792-94ACB32DB4EC}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{3E1A4BA4-A92F-724C-AE87-430A70601B53}" type="pres">
-      <dgm:prSet presAssocID="{05B6BD45-2167-C941-A792-94ACB32DB4EC}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="4" presStyleCnt="11">
+    <dgm:pt modelId="{DEA98603-1475-6643-B90D-B4C5B3BB2727}" type="pres">
+      <dgm:prSet presAssocID="{C762D9DC-C267-9446-B1CC-A95E3114C015}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5DFE3D87-3E56-EE42-9E29-FC62E4F1FBAE}" type="pres">
+      <dgm:prSet presAssocID="{41576158-B990-5740-AFD7-A7F30A9E11F8}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="4" presStyleCnt="13"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{59900680-E755-2F4D-8CBF-262A200A8D9D}" type="pres">
+      <dgm:prSet presAssocID="{41576158-B990-5740-AFD7-A7F30A9E11F8}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="4" presStyleCnt="13"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5A3C6DA5-EB5E-6B46-BC3A-243E7E9C2D82}" type="pres">
+      <dgm:prSet presAssocID="{DA4300B2-2331-2046-ABC1-100C122A715A}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{8A60DE61-E72C-854C-836C-D906D1A70AB7}" type="pres">
+      <dgm:prSet presAssocID="{DA4300B2-2331-2046-ABC1-100C122A715A}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="4" presStyleCnt="13">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2172,24 +2389,38 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{0FCCF158-7203-874A-BC78-6D0864195E77}" type="pres">
-      <dgm:prSet presAssocID="{05B6BD45-2167-C941-A792-94ACB32DB4EC}" presName="level3hierChild" presStyleCnt="0"/>
+    <dgm:pt modelId="{8EF72282-BF11-7743-901F-6D51777AFDF4}" type="pres">
+      <dgm:prSet presAssocID="{DA4300B2-2331-2046-ABC1-100C122A715A}" presName="level3hierChild" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{25F721B1-6D69-F140-A42C-4801B2DBF60A}" type="pres">
-      <dgm:prSet presAssocID="{43DE405C-0005-D145-AF97-5263D0BFD64F}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="5" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{43DE405C-0005-D145-AF97-5263D0BFD64F}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="5" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{3977402A-F54C-7B4F-97CE-88E597C91DA3}" type="pres">
-      <dgm:prSet presAssocID="{43DE405C-0005-D145-AF97-5263D0BFD64F}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="5" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{43DE405C-0005-D145-AF97-5263D0BFD64F}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="5" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{392EE4AA-6742-B242-BEC9-4763AF49A400}" type="pres">
       <dgm:prSet presAssocID="{B0BC72F6-8193-FD42-B124-F6D52726A515}" presName="root2" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{84D18324-7849-AF4F-A07E-80E004C8B650}" type="pres">
-      <dgm:prSet presAssocID="{B0BC72F6-8193-FD42-B124-F6D52726A515}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="5" presStyleCnt="11">
+      <dgm:prSet presAssocID="{B0BC72F6-8193-FD42-B124-F6D52726A515}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="5" presStyleCnt="13">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2208,19 +2439,33 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{CD750812-B108-564F-992D-C437D68E95A1}" type="pres">
-      <dgm:prSet presAssocID="{C21A12D2-AB62-2C43-BA4D-09A91CAB6E7F}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="5" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{C21A12D2-AB62-2C43-BA4D-09A91CAB6E7F}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="6" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{085C6D68-61FF-5147-81E0-9AEF37B2ECCB}" type="pres">
-      <dgm:prSet presAssocID="{C21A12D2-AB62-2C43-BA4D-09A91CAB6E7F}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="5" presStyleCnt="11"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{C21A12D2-AB62-2C43-BA4D-09A91CAB6E7F}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="6" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{AE3ABCE3-88A7-4D40-8B8A-323DD095ABDD}" type="pres">
       <dgm:prSet presAssocID="{58A735CD-359C-954E-AB8F-0259B5D1CCE7}" presName="root2" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{69AC3AD2-ED21-5344-AD1D-FDFEEE7C4C5B}" type="pres">
-      <dgm:prSet presAssocID="{58A735CD-359C-954E-AB8F-0259B5D1CCE7}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="5" presStyleCnt="11">
+      <dgm:prSet presAssocID="{58A735CD-359C-954E-AB8F-0259B5D1CCE7}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="6" presStyleCnt="13">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2238,20 +2483,20 @@
       <dgm:prSet presAssocID="{58A735CD-359C-954E-AB8F-0259B5D1CCE7}" presName="level3hierChild" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{199187A2-043D-8540-A3D5-F92622E95501}" type="pres">
-      <dgm:prSet presAssocID="{DA49E6E9-CDF9-794C-AEAB-4FBD68A57F1A}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="6" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{968DCEBD-CF0C-D74A-A666-31158F65E182}" type="pres">
-      <dgm:prSet presAssocID="{DA49E6E9-CDF9-794C-AEAB-4FBD68A57F1A}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="6" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{6C1E8FD9-477E-684D-B4BA-F9AD3239AD3B}" type="pres">
-      <dgm:prSet presAssocID="{A8AC0743-8DDE-2742-BA27-AC8B8ED11478}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{2A221514-4A03-4B45-B5AF-749FB8232375}" type="pres">
-      <dgm:prSet presAssocID="{A8AC0743-8DDE-2742-BA27-AC8B8ED11478}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="6" presStyleCnt="11">
+    <dgm:pt modelId="{11AB213E-7F90-F141-9549-20DEA56EEBBD}" type="pres">
+      <dgm:prSet presAssocID="{BE5B9591-AC80-4946-8C78-D7570297C39E}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="7" presStyleCnt="13"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C89AF06C-5711-7D48-A237-493096B9D115}" type="pres">
+      <dgm:prSet presAssocID="{BE5B9591-AC80-4946-8C78-D7570297C39E}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="7" presStyleCnt="13"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{EDD11DE7-1B17-6D40-912C-B73F3838AC65}" type="pres">
+      <dgm:prSet presAssocID="{0B970462-F13C-4D48-A4B7-10C043EEEE2B}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{080C10A4-0453-4948-B1F3-2DFE4B8C8CE4}" type="pres">
+      <dgm:prSet presAssocID="{0B970462-F13C-4D48-A4B7-10C043EEEE2B}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="7" presStyleCnt="13">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2265,24 +2510,24 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{6F7BF31D-8E73-9A4D-8E76-ECB3E38C37A1}" type="pres">
-      <dgm:prSet presAssocID="{A8AC0743-8DDE-2742-BA27-AC8B8ED11478}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{5DA24466-CB9E-0F43-B8A3-FA63AE383C78}" type="pres">
-      <dgm:prSet presAssocID="{3D9D5180-F8A4-1241-9004-FDBC86CE8EB7}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="6" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{022121AF-B706-D246-99BA-880E7AB5B05A}" type="pres">
-      <dgm:prSet presAssocID="{3D9D5180-F8A4-1241-9004-FDBC86CE8EB7}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="6" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{120D2242-86A1-A442-A1C7-C33EE729768D}" type="pres">
-      <dgm:prSet presAssocID="{C6790FB4-8208-8143-B098-50B34734D56A}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{9F55E6EF-25E4-B542-8DEE-25656226127F}" type="pres">
-      <dgm:prSet presAssocID="{C6790FB4-8208-8143-B098-50B34734D56A}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="6" presStyleCnt="11">
+    <dgm:pt modelId="{F045EA84-A9CB-8941-BD1C-77E82ACA70BC}" type="pres">
+      <dgm:prSet presAssocID="{0B970462-F13C-4D48-A4B7-10C043EEEE2B}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E4A90812-59D6-D34C-91E1-E3C466D41D1B}" type="pres">
+      <dgm:prSet presAssocID="{2E18F920-A737-724D-B818-02F6FE67E8FC}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="8" presStyleCnt="13"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{6B763081-220F-944D-96A7-37B055955D48}" type="pres">
+      <dgm:prSet presAssocID="{2E18F920-A737-724D-B818-02F6FE67E8FC}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="8" presStyleCnt="13"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{8ED44C45-8E58-4B40-B6C1-F9FAD4C31112}" type="pres">
+      <dgm:prSet presAssocID="{3E620EDA-5ADD-CC44-8C95-9FC1DF254361}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{BBEAC981-0AA3-BE43-933A-96CDBD00C9A2}" type="pres">
+      <dgm:prSet presAssocID="{3E620EDA-5ADD-CC44-8C95-9FC1DF254361}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="8" presStyleCnt="13">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2296,24 +2541,24 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{645BCC2E-DF41-B64E-8B89-6603B642452E}" type="pres">
-      <dgm:prSet presAssocID="{C6790FB4-8208-8143-B098-50B34734D56A}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{A608BD11-03C6-9149-9A0C-9460A3FE91FB}" type="pres">
-      <dgm:prSet presAssocID="{898D5F8F-CA92-7B4D-9D96-13C7CC8EB24F}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="7" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{D5068B54-DECB-5C40-8C43-3E238EA1A151}" type="pres">
-      <dgm:prSet presAssocID="{898D5F8F-CA92-7B4D-9D96-13C7CC8EB24F}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="7" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{85DB200A-1A2A-4E49-BB42-9798DD0F7491}" type="pres">
-      <dgm:prSet presAssocID="{2064DC40-2F6A-7246-96EB-B7DCB07874C8}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{D90297FE-FAC7-9042-A8CC-4C7D825B33BF}" type="pres">
-      <dgm:prSet presAssocID="{2064DC40-2F6A-7246-96EB-B7DCB07874C8}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="7" presStyleCnt="11">
+    <dgm:pt modelId="{4F1BB898-E113-A845-BCED-21337085BC33}" type="pres">
+      <dgm:prSet presAssocID="{3E620EDA-5ADD-CC44-8C95-9FC1DF254361}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{FE83888B-4547-9642-A036-470E88BA049D}" type="pres">
+      <dgm:prSet presAssocID="{E2540CE2-F2F8-7D4E-8EF4-139718573F86}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="9" presStyleCnt="13"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{A77D1BEF-37F9-7242-91A8-9D907E7CC0B4}" type="pres">
+      <dgm:prSet presAssocID="{E2540CE2-F2F8-7D4E-8EF4-139718573F86}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="9" presStyleCnt="13"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{DC1F6217-0341-D948-9642-F637E5F7E362}" type="pres">
+      <dgm:prSet presAssocID="{30615BCE-5A85-DD4B-B246-1B251E40150B}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{567E4FBD-1A65-6B48-8A6D-F72A7955CE15}" type="pres">
+      <dgm:prSet presAssocID="{30615BCE-5A85-DD4B-B246-1B251E40150B}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="9" presStyleCnt="13">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2327,24 +2572,38 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{43967FCB-616D-F84C-8966-503D83458021}" type="pres">
-      <dgm:prSet presAssocID="{2064DC40-2F6A-7246-96EB-B7DCB07874C8}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{96B1CDE0-C35A-CB43-9A64-AE7BDFB44B3E}" type="pres">
-      <dgm:prSet presAssocID="{4FDA31E9-0995-E646-B247-48C734F29F55}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="7" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{769BF5E9-2773-7642-A2AF-516B0418FC0F}" type="pres">
-      <dgm:prSet presAssocID="{4FDA31E9-0995-E646-B247-48C734F29F55}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="7" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{BA13AD0C-76AA-5843-A605-E16AAE70ED9A}" type="pres">
-      <dgm:prSet presAssocID="{94300211-45FB-9547-B995-E1E57425CDE7}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{9FDC99B0-D551-004A-864C-6DCAFEB88B76}" type="pres">
-      <dgm:prSet presAssocID="{94300211-45FB-9547-B995-E1E57425CDE7}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="7" presStyleCnt="11">
+    <dgm:pt modelId="{4064B30A-9269-F742-B21A-E7536FBB9B43}" type="pres">
+      <dgm:prSet presAssocID="{30615BCE-5A85-DD4B-B246-1B251E40150B}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{199187A2-043D-8540-A3D5-F92622E95501}" type="pres">
+      <dgm:prSet presAssocID="{DA49E6E9-CDF9-794C-AEAB-4FBD68A57F1A}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="5" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{968DCEBD-CF0C-D74A-A666-31158F65E182}" type="pres">
+      <dgm:prSet presAssocID="{DA49E6E9-CDF9-794C-AEAB-4FBD68A57F1A}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="5" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{6C1E8FD9-477E-684D-B4BA-F9AD3239AD3B}" type="pres">
+      <dgm:prSet presAssocID="{A8AC0743-8DDE-2742-BA27-AC8B8ED11478}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{2A221514-4A03-4B45-B5AF-749FB8232375}" type="pres">
+      <dgm:prSet presAssocID="{A8AC0743-8DDE-2742-BA27-AC8B8ED11478}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="5" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2358,24 +2617,38 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{F767CC2E-1D10-8745-9E1F-96823794A4C7}" type="pres">
-      <dgm:prSet presAssocID="{94300211-45FB-9547-B995-E1E57425CDE7}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{49C1BB80-7116-0243-8559-F49FE35EAC8C}" type="pres">
-      <dgm:prSet presAssocID="{A3EE15A6-3F32-E047-A7C8-658B5B9A2426}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="8" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{7DED3A20-7857-564A-9D1E-9551D5E2DF6D}" type="pres">
-      <dgm:prSet presAssocID="{A3EE15A6-3F32-E047-A7C8-658B5B9A2426}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="8" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{9289C2FC-A477-3647-940B-134169176A90}" type="pres">
-      <dgm:prSet presAssocID="{E1246F00-5110-6146-85B3-F18EAD31DE44}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{96296898-BE98-0247-83BE-61F5D3D682F5}" type="pres">
-      <dgm:prSet presAssocID="{E1246F00-5110-6146-85B3-F18EAD31DE44}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="8" presStyleCnt="11">
+    <dgm:pt modelId="{6F7BF31D-8E73-9A4D-8E76-ECB3E38C37A1}" type="pres">
+      <dgm:prSet presAssocID="{A8AC0743-8DDE-2742-BA27-AC8B8ED11478}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5DA24466-CB9E-0F43-B8A3-FA63AE383C78}" type="pres">
+      <dgm:prSet presAssocID="{3D9D5180-F8A4-1241-9004-FDBC86CE8EB7}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="10" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{022121AF-B706-D246-99BA-880E7AB5B05A}" type="pres">
+      <dgm:prSet presAssocID="{3D9D5180-F8A4-1241-9004-FDBC86CE8EB7}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="10" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{120D2242-86A1-A442-A1C7-C33EE729768D}" type="pres">
+      <dgm:prSet presAssocID="{C6790FB4-8208-8143-B098-50B34734D56A}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{9F55E6EF-25E4-B542-8DEE-25656226127F}" type="pres">
+      <dgm:prSet presAssocID="{C6790FB4-8208-8143-B098-50B34734D56A}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="10" presStyleCnt="13">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2389,24 +2662,24 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{845FD99B-46AA-D04B-996F-EFB1B6DC0135}" type="pres">
-      <dgm:prSet presAssocID="{E1246F00-5110-6146-85B3-F18EAD31DE44}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{04C15EBF-48BF-2D4C-BF9B-0823F14313EF}" type="pres">
-      <dgm:prSet presAssocID="{98BE4178-0B33-D54A-91F1-7CD2B3AC77E2}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="8" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{C08397E8-4357-1040-B413-6547DDCD0CDD}" type="pres">
-      <dgm:prSet presAssocID="{98BE4178-0B33-D54A-91F1-7CD2B3AC77E2}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="8" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{1DED0AA9-3924-334A-8D8D-33478E7657B0}" type="pres">
-      <dgm:prSet presAssocID="{1FCD6FA2-2EC1-E044-8817-90704567D52F}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{98E56F84-7B9F-E448-A77F-BECF084C032C}" type="pres">
-      <dgm:prSet presAssocID="{1FCD6FA2-2EC1-E044-8817-90704567D52F}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="8" presStyleCnt="11">
+    <dgm:pt modelId="{645BCC2E-DF41-B64E-8B89-6603B642452E}" type="pres">
+      <dgm:prSet presAssocID="{C6790FB4-8208-8143-B098-50B34734D56A}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{622176D4-0F63-4441-9655-4E39F2D4E064}" type="pres">
+      <dgm:prSet presAssocID="{FA9F03C1-DE3A-9849-9BB9-A7264514AC98}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="4"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{9CBE3C3D-6969-BA40-9AFD-12D8A930CA33}" type="pres">
+      <dgm:prSet presAssocID="{FA9F03C1-DE3A-9849-9BB9-A7264514AC98}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="4"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{4F9608FB-4CF1-644A-A181-4483BAED8A3B}" type="pres">
+      <dgm:prSet presAssocID="{652DE9CE-379E-5542-8267-C153E850CFF5}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F9CE8C8D-1F59-A546-857D-5DCA77549F01}" type="pres">
+      <dgm:prSet presAssocID="{652DE9CE-379E-5542-8267-C153E850CFF5}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="2" presStyleCnt="4">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2420,24 +2693,24 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{4F99EDBC-C258-2349-A0FD-89D18599CDD0}" type="pres">
-      <dgm:prSet presAssocID="{1FCD6FA2-2EC1-E044-8817-90704567D52F}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{F2B8E9EC-9E8D-EF4F-8069-8CF8FD8833B2}" type="pres">
-      <dgm:prSet presAssocID="{DE6250AC-E2C3-EA4C-90F4-F144D5C45412}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="3"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{1A86F6FD-7823-CA48-AB5A-F31345841067}" type="pres">
-      <dgm:prSet presAssocID="{DE6250AC-E2C3-EA4C-90F4-F144D5C45412}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="3"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{D5E11BF9-817C-CD42-900E-A9BC452624B0}" type="pres">
-      <dgm:prSet presAssocID="{EB608E93-0479-2148-BCC1-5BA22B50A826}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{53EE5430-A405-0C45-8C3D-56B9B7B4C5EE}" type="pres">
-      <dgm:prSet presAssocID="{EB608E93-0479-2148-BCC1-5BA22B50A826}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="2" presStyleCnt="3">
+    <dgm:pt modelId="{EB59BBE9-3A43-2145-809F-98F8ECA7D98F}" type="pres">
+      <dgm:prSet presAssocID="{652DE9CE-379E-5542-8267-C153E850CFF5}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{EC671750-0F9F-144E-B9B1-0F71732606F0}" type="pres">
+      <dgm:prSet presAssocID="{F97D5CCC-FB1C-BD4D-8FC0-8444F262955E}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="6" presStyleCnt="10"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{56D4E8B8-277E-6C4C-B5C0-2B77C4634751}" type="pres">
+      <dgm:prSet presAssocID="{F97D5CCC-FB1C-BD4D-8FC0-8444F262955E}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="6" presStyleCnt="10"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{568918D7-6938-E249-9E2B-254463D3E59B}" type="pres">
+      <dgm:prSet presAssocID="{6DC6F20A-841D-E944-B9FD-E1D140F60C2C}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{DFF22F0D-7EB3-DB46-B99E-239BB764C2DC}" type="pres">
+      <dgm:prSet presAssocID="{6DC6F20A-841D-E944-B9FD-E1D140F60C2C}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="6" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2451,24 +2724,24 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{0B0444E0-1C9D-7944-896B-7915BA26BAB2}" type="pres">
-      <dgm:prSet presAssocID="{EB608E93-0479-2148-BCC1-5BA22B50A826}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{CF5C0BC9-1C55-6D44-9740-9A1957FD4485}" type="pres">
-      <dgm:prSet presAssocID="{8F42AAD0-AA72-224D-89F6-60847A76B1D5}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="9" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{C1AA1D1D-23B3-5348-98C0-620CC9C417E7}" type="pres">
-      <dgm:prSet presAssocID="{8F42AAD0-AA72-224D-89F6-60847A76B1D5}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="9" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{6D9D35C7-1C29-A94A-9481-8C3259586318}" type="pres">
-      <dgm:prSet presAssocID="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{8F0E1068-96D7-094C-A746-F91F87169C20}" type="pres">
-      <dgm:prSet presAssocID="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="9" presStyleCnt="11">
+    <dgm:pt modelId="{F519F3D3-72EC-D546-97C3-75849C2CA254}" type="pres">
+      <dgm:prSet presAssocID="{6DC6F20A-841D-E944-B9FD-E1D140F60C2C}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{9FA40A36-B6C2-5140-97C1-947018A2B70F}" type="pres">
+      <dgm:prSet presAssocID="{551B3FB5-3F7C-9046-B05E-7E0316CCFFDC}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="7" presStyleCnt="10"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5E4F97FA-974D-8845-A8FE-60389B8C4834}" type="pres">
+      <dgm:prSet presAssocID="{551B3FB5-3F7C-9046-B05E-7E0316CCFFDC}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="7" presStyleCnt="10"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C0072E1F-3A0C-0940-A1CD-530FB2B10CD1}" type="pres">
+      <dgm:prSet presAssocID="{5E402F45-6CF9-7D49-9393-47131AFD7CE6}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{0963A656-C5DC-AB41-8DEE-D65A14EA566F}" type="pres">
+      <dgm:prSet presAssocID="{5E402F45-6CF9-7D49-9393-47131AFD7CE6}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="7" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2482,24 +2755,38 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{001EB529-925E-D549-9ADD-044F795FEF21}" type="pres">
-      <dgm:prSet presAssocID="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{78144F12-25BE-F943-8DB8-4D280CF8337F}" type="pres">
-      <dgm:prSet presAssocID="{48D60804-A609-D344-B265-30D430B4E428}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="9" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{2B0D2414-9C87-0445-8FBF-CB229BF7118E}" type="pres">
-      <dgm:prSet presAssocID="{48D60804-A609-D344-B265-30D430B4E428}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="9" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{A5B42E29-B28A-8D4D-B5BA-419E461A3E50}" type="pres">
-      <dgm:prSet presAssocID="{9756178B-0C1F-AA4C-B73B-5C8C2B47A9E1}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{EC0EB3A7-6AD7-5242-97AF-E79A69522BAB}" type="pres">
-      <dgm:prSet presAssocID="{9756178B-0C1F-AA4C-B73B-5C8C2B47A9E1}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="9" presStyleCnt="11">
+    <dgm:pt modelId="{63BE4F91-CBE1-B542-8CD4-1BA6649119A2}" type="pres">
+      <dgm:prSet presAssocID="{5E402F45-6CF9-7D49-9393-47131AFD7CE6}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F2B8E9EC-9E8D-EF4F-8069-8CF8FD8833B2}" type="pres">
+      <dgm:prSet presAssocID="{DE6250AC-E2C3-EA4C-90F4-F144D5C45412}" presName="conn2-1" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="4"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{1A86F6FD-7823-CA48-AB5A-F31345841067}" type="pres">
+      <dgm:prSet presAssocID="{DE6250AC-E2C3-EA4C-90F4-F144D5C45412}" presName="connTx" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="4"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{D5E11BF9-817C-CD42-900E-A9BC452624B0}" type="pres">
+      <dgm:prSet presAssocID="{EB608E93-0479-2148-BCC1-5BA22B50A826}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{53EE5430-A405-0C45-8C3D-56B9B7B4C5EE}" type="pres">
+      <dgm:prSet presAssocID="{EB608E93-0479-2148-BCC1-5BA22B50A826}" presName="LevelTwoTextNode" presStyleLbl="node2" presStyleIdx="3" presStyleCnt="4">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2513,24 +2800,38 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{91FB988E-5182-EF44-A9B3-6BE7162C4F5D}" type="pres">
-      <dgm:prSet presAssocID="{9756178B-0C1F-AA4C-B73B-5C8C2B47A9E1}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{48799966-5966-574A-BC3A-266F4C6BAF17}" type="pres">
-      <dgm:prSet presAssocID="{0FCF08F7-3C86-6A4A-965A-08D4C71F2C83}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="10" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{9C06130D-D3CF-6C4B-9249-8865DD724342}" type="pres">
-      <dgm:prSet presAssocID="{0FCF08F7-3C86-6A4A-965A-08D4C71F2C83}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="10" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{06C7D346-37EA-A348-AFEB-EBF697672BFC}" type="pres">
-      <dgm:prSet presAssocID="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{8DA6C1C2-E0BE-DE44-8DDE-6C55EBB1BE40}" type="pres">
-      <dgm:prSet presAssocID="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="10" presStyleCnt="11">
+    <dgm:pt modelId="{0B0444E0-1C9D-7944-896B-7915BA26BAB2}" type="pres">
+      <dgm:prSet presAssocID="{EB608E93-0479-2148-BCC1-5BA22B50A826}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{CF5C0BC9-1C55-6D44-9740-9A1957FD4485}" type="pres">
+      <dgm:prSet presAssocID="{8F42AAD0-AA72-224D-89F6-60847A76B1D5}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="8" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C1AA1D1D-23B3-5348-98C0-620CC9C417E7}" type="pres">
+      <dgm:prSet presAssocID="{8F42AAD0-AA72-224D-89F6-60847A76B1D5}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="8" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{6D9D35C7-1C29-A94A-9481-8C3259586318}" type="pres">
+      <dgm:prSet presAssocID="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{8F0E1068-96D7-094C-A746-F91F87169C20}" type="pres">
+      <dgm:prSet presAssocID="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="8" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2544,24 +2845,38 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{05EF386D-5FC3-074D-B632-6D765D3A5770}" type="pres">
-      <dgm:prSet presAssocID="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}" presName="level3hierChild" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{8767306D-9113-BC4B-81AA-7FB530A91291}" type="pres">
-      <dgm:prSet presAssocID="{898657C8-0B6D-224B-8CFB-19156D73C9DA}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="10" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{8E9E86BF-4214-C04F-819A-80928C1A4988}" type="pres">
-      <dgm:prSet presAssocID="{898657C8-0B6D-224B-8CFB-19156D73C9DA}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="10" presStyleCnt="11"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{ECC8294F-FFE7-924F-8175-82D5C5652EC5}" type="pres">
-      <dgm:prSet presAssocID="{9DF1FBC3-19A9-8348-954D-040117F5C5B6}" presName="root2" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{8B5EE93D-B5D5-D545-9E38-B095AB10F5BE}" type="pres">
-      <dgm:prSet presAssocID="{9DF1FBC3-19A9-8348-954D-040117F5C5B6}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="10" presStyleCnt="11">
+    <dgm:pt modelId="{001EB529-925E-D549-9ADD-044F795FEF21}" type="pres">
+      <dgm:prSet presAssocID="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{78144F12-25BE-F943-8DB8-4D280CF8337F}" type="pres">
+      <dgm:prSet presAssocID="{48D60804-A609-D344-B265-30D430B4E428}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="11" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{2B0D2414-9C87-0445-8FBF-CB229BF7118E}" type="pres">
+      <dgm:prSet presAssocID="{48D60804-A609-D344-B265-30D430B4E428}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="11" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{A5B42E29-B28A-8D4D-B5BA-419E461A3E50}" type="pres">
+      <dgm:prSet presAssocID="{9756178B-0C1F-AA4C-B73B-5C8C2B47A9E1}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{EC0EB3A7-6AD7-5242-97AF-E79A69522BAB}" type="pres">
+      <dgm:prSet presAssocID="{9756178B-0C1F-AA4C-B73B-5C8C2B47A9E1}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="11" presStyleCnt="13">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2575,115 +2890,213 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
+    <dgm:pt modelId="{91FB988E-5182-EF44-A9B3-6BE7162C4F5D}" type="pres">
+      <dgm:prSet presAssocID="{9756178B-0C1F-AA4C-B73B-5C8C2B47A9E1}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{48799966-5966-574A-BC3A-266F4C6BAF17}" type="pres">
+      <dgm:prSet presAssocID="{0FCF08F7-3C86-6A4A-965A-08D4C71F2C83}" presName="conn2-1" presStyleLbl="parChTrans1D3" presStyleIdx="9" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{9C06130D-D3CF-6C4B-9249-8865DD724342}" type="pres">
+      <dgm:prSet presAssocID="{0FCF08F7-3C86-6A4A-965A-08D4C71F2C83}" presName="connTx" presStyleLbl="parChTrans1D3" presStyleIdx="9" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{06C7D346-37EA-A348-AFEB-EBF697672BFC}" type="pres">
+      <dgm:prSet presAssocID="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{8DA6C1C2-E0BE-DE44-8DDE-6C55EBB1BE40}" type="pres">
+      <dgm:prSet presAssocID="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}" presName="LevelTwoTextNode" presStyleLbl="node3" presStyleIdx="9" presStyleCnt="10">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{05EF386D-5FC3-074D-B632-6D765D3A5770}" type="pres">
+      <dgm:prSet presAssocID="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}" presName="level3hierChild" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{8767306D-9113-BC4B-81AA-7FB530A91291}" type="pres">
+      <dgm:prSet presAssocID="{898657C8-0B6D-224B-8CFB-19156D73C9DA}" presName="conn2-1" presStyleLbl="parChTrans1D4" presStyleIdx="12" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{8E9E86BF-4214-C04F-819A-80928C1A4988}" type="pres">
+      <dgm:prSet presAssocID="{898657C8-0B6D-224B-8CFB-19156D73C9DA}" presName="connTx" presStyleLbl="parChTrans1D4" presStyleIdx="12" presStyleCnt="13"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{ECC8294F-FFE7-924F-8175-82D5C5652EC5}" type="pres">
+      <dgm:prSet presAssocID="{9DF1FBC3-19A9-8348-954D-040117F5C5B6}" presName="root2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{8B5EE93D-B5D5-D545-9E38-B095AB10F5BE}" type="pres">
+      <dgm:prSet presAssocID="{9DF1FBC3-19A9-8348-954D-040117F5C5B6}" presName="LevelTwoTextNode" presStyleLbl="node4" presStyleIdx="12" presStyleCnt="13">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
     <dgm:pt modelId="{7814CF00-83DE-0B4C-B23D-F025D6F6C2C5}" type="pres">
       <dgm:prSet presAssocID="{9DF1FBC3-19A9-8348-954D-040117F5C5B6}" presName="level3hierChild" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
+    <dgm:cxn modelId="{3348C0B5-1D0A-6E45-891C-EA5721A2DED7}" type="presOf" srcId="{0749699B-B7C4-6140-B4CB-8D60FBCE1ECB}" destId="{36C0C19B-3F9B-2049-BB73-D3B74079B1BA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{2A628D16-EE35-924F-9FD4-D158B6311FBA}" type="presOf" srcId="{FA9F03C1-DE3A-9849-9BB9-A7264514AC98}" destId="{622176D4-0F63-4441-9655-4E39F2D4E064}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{7DB2C1AF-3B5B-7C43-854C-BF3A2DB639BA}" srcId="{3D5AE65B-9194-A04D-98AC-695DC8D2BA16}" destId="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" srcOrd="0" destOrd="0" parTransId="{66816B50-209E-8A44-99FF-FCA0FE6010CF}" sibTransId="{003A5410-B948-1B4C-AECA-2D523EED1A72}"/>
+    <dgm:cxn modelId="{894FAB9C-376D-744F-A028-9D417D5EC8DD}" type="presOf" srcId="{14BF84F4-E713-F349-BD2A-D68DD017694A}" destId="{CB5AFF4C-0CEC-F643-96B6-DAC4ED874BEC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{A2083FBA-858C-D94E-8CD7-6E332E9BFC97}" type="presOf" srcId="{2E18F920-A737-724D-B818-02F6FE67E8FC}" destId="{E4A90812-59D6-D34C-91E1-E3C466D41D1B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{F200E26E-0AA3-104C-A445-0A16851EF130}" type="presOf" srcId="{8F42AAD0-AA72-224D-89F6-60847A76B1D5}" destId="{CF5C0BC9-1C55-6D44-9740-9A1957FD4485}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{C2E8BEEA-6AB0-1540-BCA7-7D857D0EE50A}" type="presOf" srcId="{63E4C9E5-BCE9-274B-B154-D1722539B787}" destId="{E51D49A7-6AFC-F04F-9B53-612EDC5C173D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{98E934AA-ECF6-7241-A5BD-70E64D2B430F}" type="presOf" srcId="{D98F1744-A7D7-C14A-B6A1-DD15D46D8107}" destId="{2060447F-F68C-B74F-BF84-BB6A544B165A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{4C26807E-41C6-BD4F-98C8-C78B73CB3A48}" srcId="{36BBC7EB-D363-3B48-8496-AA60D47185CD}" destId="{B1871CE9-AA57-7E40-9F44-89545C773C31}" srcOrd="0" destOrd="0" parTransId="{3F5EFC20-7888-8B4C-A3B9-D9A3746FD5D9}" sibTransId="{5D8571E4-D1F1-6648-B5D0-EB4F7F948761}"/>
+    <dgm:cxn modelId="{714AF0CD-13D5-5241-9539-5CA4808D0AD3}" type="presOf" srcId="{3D5AE65B-9194-A04D-98AC-695DC8D2BA16}" destId="{61D69160-A7CD-9049-954F-FA5CBF774AED}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{CCBF3526-4864-E04B-9D46-0753A6E98C06}" type="presOf" srcId="{551B3FB5-3F7C-9046-B05E-7E0316CCFFDC}" destId="{9FA40A36-B6C2-5140-97C1-947018A2B70F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{782DD2D0-5D5C-0F43-9983-36421DC4FA94}" type="presOf" srcId="{3D9D5180-F8A4-1241-9004-FDBC86CE8EB7}" destId="{022121AF-B706-D246-99BA-880E7AB5B05A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{87500F0C-3129-4043-A941-9960C7FDFE5F}" srcId="{C762D9DC-C267-9446-B1CC-A95E3114C015}" destId="{0B970462-F13C-4D48-A4B7-10C043EEEE2B}" srcOrd="2" destOrd="0" parTransId="{BE5B9591-AC80-4946-8C78-D7570297C39E}" sibTransId="{9C7B62F8-4A99-4948-9007-9C010A739C17}"/>
+    <dgm:cxn modelId="{B88C949E-BE70-6646-B154-E56E02AA7AD8}" type="presOf" srcId="{3F5EFC20-7888-8B4C-A3B9-D9A3746FD5D9}" destId="{61A4E688-2EE9-2949-9B58-3693E86C97FB}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{844E2698-F22A-D343-AB95-197D90F2F9D0}" srcId="{3D5AE65B-9194-A04D-98AC-695DC8D2BA16}" destId="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" srcOrd="1" destOrd="0" parTransId="{BC4BC998-E1F0-5B45-A719-663711F9FB23}" sibTransId="{DDB0B02F-B0F4-F846-A7E4-E7A12917CEB3}"/>
+    <dgm:cxn modelId="{06FADF7B-BEC5-7C43-994B-AC10C0BB5165}" type="presOf" srcId="{3D9D5180-F8A4-1241-9004-FDBC86CE8EB7}" destId="{5DA24466-CB9E-0F43-B8A3-FA63AE383C78}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{57B49347-DDE9-3943-BD16-CE8F3969BDEF}" type="presOf" srcId="{48D60804-A609-D344-B265-30D430B4E428}" destId="{2B0D2414-9C87-0445-8FBF-CB229BF7118E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{6B22011B-E30A-C543-ADD5-8BD1F8C3B793}" type="presOf" srcId="{30615BCE-5A85-DD4B-B246-1B251E40150B}" destId="{567E4FBD-1A65-6B48-8A6D-F72A7955CE15}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{7B6DC8CC-26FA-7A40-BD86-B1BD62DED8AA}" type="presOf" srcId="{36BBC7EB-D363-3B48-8496-AA60D47185CD}" destId="{E51D9155-7752-9D41-957A-949CC75EB761}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{A88E5FD2-A613-7B4D-B5C5-FADE7864F541}" type="presOf" srcId="{66816B50-209E-8A44-99FF-FCA0FE6010CF}" destId="{2680328F-7469-384B-A713-47DAA1730724}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{7D5B75CF-0F32-2E4A-8660-0FF6CF30448C}" type="presOf" srcId="{8F5969EE-F8BE-0348-8A1D-523AF7ADC449}" destId="{ED82EB34-8097-994C-90F2-D4621919418A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{21EA7D0D-133A-A944-A6F7-101660CD2A30}" type="presOf" srcId="{E2540CE2-F2F8-7D4E-8EF4-139718573F86}" destId="{A77D1BEF-37F9-7242-91A8-9D907E7CC0B4}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{507C37D9-DF70-C049-AB45-6D6194C6EDD1}" srcId="{3D5AE65B-9194-A04D-98AC-695DC8D2BA16}" destId="{EB608E93-0479-2148-BCC1-5BA22B50A826}" srcOrd="3" destOrd="0" parTransId="{DE6250AC-E2C3-EA4C-90F4-F144D5C45412}" sibTransId="{873FE768-EBDB-5444-A928-15F6A44CCEAB}"/>
+    <dgm:cxn modelId="{98306D63-FFBF-4B41-847D-6CAC1EA77F57}" srcId="{CBD00C11-7705-4B46-A507-504E11D7B2C4}" destId="{05B6BD45-2167-C941-A792-94ACB32DB4EC}" srcOrd="0" destOrd="0" parTransId="{D98F1744-A7D7-C14A-B6A1-DD15D46D8107}" sibTransId="{41378A21-F6F6-AC47-B392-C0CCEED89946}"/>
+    <dgm:cxn modelId="{7BDF0CB4-4494-3841-A0C2-B96746C922B8}" srcId="{EB608E93-0479-2148-BCC1-5BA22B50A826}" destId="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}" srcOrd="0" destOrd="0" parTransId="{8F42AAD0-AA72-224D-89F6-60847A76B1D5}" sibTransId="{C3BA1502-7EEB-0B4D-89AF-D304786068A6}"/>
+    <dgm:cxn modelId="{6E431DE5-A5CB-904E-AC51-9908AD548198}" srcId="{8F5969EE-F8BE-0348-8A1D-523AF7ADC449}" destId="{2F71905B-FED7-7946-BB13-3426F23C1911}" srcOrd="0" destOrd="0" parTransId="{0749699B-B7C4-6140-B4CB-8D60FBCE1ECB}" sibTransId="{DA70BC87-3097-4A43-94C7-A082FCE90909}"/>
+    <dgm:cxn modelId="{63BA776F-0A66-AD46-B623-5776CE9A8700}" type="presOf" srcId="{BE5B9591-AC80-4946-8C78-D7570297C39E}" destId="{C89AF06C-5711-7D48-A237-493096B9D115}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{935CFD64-B563-C14A-8843-98A8FBBCCE52}" srcId="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" destId="{C762D9DC-C267-9446-B1CC-A95E3114C015}" srcOrd="1" destOrd="0" parTransId="{B5D4559E-723E-D842-BB45-358E2F203970}" sibTransId="{DA64E6F3-5664-5A48-B5C2-B7239FD965F9}"/>
+    <dgm:cxn modelId="{1C81621C-E44B-8C43-A258-03B24FAC54F1}" type="presOf" srcId="{30FE5FD2-03E7-C142-AA91-76709434DD90}" destId="{22159CD9-4EC1-E544-98E6-9AD9F99F03AF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{751DFE1C-CFA6-BB4D-9A10-F5723CA5A01D}" type="presOf" srcId="{898657C8-0B6D-224B-8CFB-19156D73C9DA}" destId="{8E9E86BF-4214-C04F-819A-80928C1A4988}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{1C512F6D-FBAA-3B49-B60D-E5DFB50B2A87}" type="presOf" srcId="{6C230476-3D0D-474F-94E9-0E58DDAF8AF5}" destId="{E462CEA6-69E8-2346-9B02-3EDF954B7021}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{614239BF-489C-314A-BFB8-FE83F3615385}" type="presOf" srcId="{551B3FB5-3F7C-9046-B05E-7E0316CCFFDC}" destId="{5E4F97FA-974D-8845-A8FE-60389B8C4834}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{CE301E01-2C61-1446-ACAA-DDD710CBC21B}" type="presOf" srcId="{DE6250AC-E2C3-EA4C-90F4-F144D5C45412}" destId="{F2B8E9EC-9E8D-EF4F-8069-8CF8FD8833B2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{E0FA02E1-0C9E-5741-B722-4FF2428F452F}" type="presOf" srcId="{B1871CE9-AA57-7E40-9F44-89545C773C31}" destId="{09A02069-0039-4049-80CB-8B6C97B26549}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{2EF8496E-B539-E644-8A60-936BF07D0C80}" type="presOf" srcId="{58A735CD-359C-954E-AB8F-0259B5D1CCE7}" destId="{69AC3AD2-ED21-5344-AD1D-FDFEEE7C4C5B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{7D2CB5FB-2947-6944-B2CF-3F1126D5C29C}" type="presOf" srcId="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" destId="{B895C344-133F-4340-80A0-685E27E999D6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{E5F81167-C364-1545-A7C5-95F0D760BF63}" srcId="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" destId="{36BBC7EB-D363-3B48-8496-AA60D47185CD}" srcOrd="0" destOrd="0" parTransId="{300BDE9E-F0C8-E145-A198-C90D0EF8BD49}" sibTransId="{47991693-D9A7-9441-8FBC-ECF07DA73E6A}"/>
+    <dgm:cxn modelId="{684E744E-37CF-B14E-BC3F-1EB3F048D34E}" type="presOf" srcId="{300BDE9E-F0C8-E145-A198-C90D0EF8BD49}" destId="{97838F66-388F-334E-8C48-6883CD119D60}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{0E9A348A-EA3F-444C-BFA5-13469C10E39B}" type="presOf" srcId="{898657C8-0B6D-224B-8CFB-19156D73C9DA}" destId="{8767306D-9113-BC4B-81AA-7FB530A91291}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{DCAEB176-E0ED-2840-9D0F-966856FBF6F5}" type="presOf" srcId="{A8AC0743-8DDE-2742-BA27-AC8B8ED11478}" destId="{2A221514-4A03-4B45-B5AF-749FB8232375}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{8D556AFB-ACA5-3343-A108-43E4822246B8}" type="presOf" srcId="{0FCF08F7-3C86-6A4A-965A-08D4C71F2C83}" destId="{48799966-5966-574A-BC3A-266F4C6BAF17}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{42FDA32E-A0D0-3C47-A7C4-1B51C6B7C1D8}" type="presOf" srcId="{C6790FB4-8208-8143-B098-50B34734D56A}" destId="{9F55E6EF-25E4-B542-8DEE-25656226127F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{2EEE2BD1-72AF-F049-923B-F0FEE359F9E1}" type="presOf" srcId="{C762D9DC-C267-9446-B1CC-A95E3114C015}" destId="{C6AA8951-971D-8D46-A6B7-A3287247CC64}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{D6930998-39E1-384C-AE5F-0FCC4707482C}" type="presOf" srcId="{B5D4559E-723E-D842-BB45-358E2F203970}" destId="{D4F4059E-9072-DD44-9070-1FDB3E4A368D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{6805E153-C0A4-F14B-8B2F-2FCE6F5E858B}" type="presOf" srcId="{0FCF08F7-3C86-6A4A-965A-08D4C71F2C83}" destId="{9C06130D-D3CF-6C4B-9249-8865DD724342}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{DB1423D0-A323-1243-91E9-AC1BD456CF7F}" type="presOf" srcId="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" destId="{02E0FECA-2589-C94E-8421-1373276E6CD0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{32F68E96-4401-3C41-932F-35D7D240B538}" srcId="{652DE9CE-379E-5542-8267-C153E850CFF5}" destId="{5E402F45-6CF9-7D49-9393-47131AFD7CE6}" srcOrd="1" destOrd="0" parTransId="{551B3FB5-3F7C-9046-B05E-7E0316CCFFDC}" sibTransId="{9798B304-7A19-9E4B-9BF5-6944B6DC86F3}"/>
+    <dgm:cxn modelId="{83885AFA-C269-8B44-8304-7BCE21B6599B}" type="presOf" srcId="{E2540CE2-F2F8-7D4E-8EF4-139718573F86}" destId="{FE83888B-4547-9642-A036-470E88BA049D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{51484080-27B2-7140-96E7-653497DA9A5F}" type="presOf" srcId="{F97D5CCC-FB1C-BD4D-8FC0-8444F262955E}" destId="{EC671750-0F9F-144E-B9B1-0F71732606F0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{115A2ACF-7A94-D043-9F9C-BD43963F59D0}" type="presOf" srcId="{C21A12D2-AB62-2C43-BA4D-09A91CAB6E7F}" destId="{CD750812-B108-564F-992D-C437D68E95A1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{697256F2-0959-D540-BCDB-AA2F49ED2902}" type="presOf" srcId="{DA4300B2-2331-2046-ABC1-100C122A715A}" destId="{8A60DE61-E72C-854C-836C-D906D1A70AB7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{8F1C49EE-1DF5-AE4D-9F7A-408782E8D8FD}" type="presOf" srcId="{63E4C9E5-BCE9-274B-B154-D1722539B787}" destId="{EC1947AE-4E19-6545-8360-1E46FEF87CE8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{E5A2EB47-D342-B941-A52E-C9F38CB342A7}" srcId="{C762D9DC-C267-9446-B1CC-A95E3114C015}" destId="{30615BCE-5A85-DD4B-B246-1B251E40150B}" srcOrd="4" destOrd="0" parTransId="{E2540CE2-F2F8-7D4E-8EF4-139718573F86}" sibTransId="{A7ADF9D2-AE55-6249-BF7E-757C29AF0CBB}"/>
+    <dgm:cxn modelId="{EDA62F54-5E8C-8547-BC49-10FD32A1CBD0}" type="presOf" srcId="{B0BC72F6-8193-FD42-B124-F6D52726A515}" destId="{84D18324-7849-AF4F-A07E-80E004C8B650}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{28FD05AD-72D6-3342-B0A7-A596896C8656}" type="presOf" srcId="{14BF84F4-E713-F349-BD2A-D68DD017694A}" destId="{BCF273FF-CB93-044A-911C-F34C18ABCD3F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{7D6DE11C-6A19-3A4D-BB4D-CAA7B0ABA0DA}" srcId="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" destId="{30FE5FD2-03E7-C142-AA91-76709434DD90}" srcOrd="1" destOrd="0" parTransId="{DC9CCC13-49B8-F64C-B46E-A357D3F309D5}" sibTransId="{749523E1-DB0A-7740-9A56-5B4F05E26FCB}"/>
+    <dgm:cxn modelId="{56D695B1-E3AA-3541-85E2-CB6032787A20}" srcId="{A8AC0743-8DDE-2742-BA27-AC8B8ED11478}" destId="{C6790FB4-8208-8143-B098-50B34734D56A}" srcOrd="0" destOrd="0" parTransId="{3D9D5180-F8A4-1241-9004-FDBC86CE8EB7}" sibTransId="{9684E716-804F-5841-98EA-1142E391B6CA}"/>
+    <dgm:cxn modelId="{208AF81C-E7E9-5E47-916E-277546BC2951}" type="presOf" srcId="{DE6250AC-E2C3-EA4C-90F4-F144D5C45412}" destId="{1A86F6FD-7823-CA48-AB5A-F31345841067}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{0B26826A-375D-AC47-A747-EF197FCFC3DA}" type="presOf" srcId="{8F42AAD0-AA72-224D-89F6-60847A76B1D5}" destId="{C1AA1D1D-23B3-5348-98C0-620CC9C417E7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{35E19FD6-62B7-8F49-8A6C-46141C8170F3}" srcId="{3D5AE65B-9194-A04D-98AC-695DC8D2BA16}" destId="{652DE9CE-379E-5542-8267-C153E850CFF5}" srcOrd="2" destOrd="0" parTransId="{FA9F03C1-DE3A-9849-9BB9-A7264514AC98}" sibTransId="{CC539F88-89BB-FB4D-9B01-F4D04CA5A22B}"/>
+    <dgm:cxn modelId="{45E47C86-8389-674E-83D8-D62646AE2199}" type="presOf" srcId="{652DE9CE-379E-5542-8267-C153E850CFF5}" destId="{F9CE8C8D-1F59-A546-857D-5DCA77549F01}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{FAD4E27E-7634-4C41-AFC9-613882ABFD95}" type="presOf" srcId="{FA9F03C1-DE3A-9849-9BB9-A7264514AC98}" destId="{9CBE3C3D-6969-BA40-9AFD-12D8A930CA33}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{AB312320-284C-6A44-ACA0-F236A55AA413}" type="presOf" srcId="{CBD00C11-7705-4B46-A507-504E11D7B2C4}" destId="{D0686948-65B5-CE4B-99C1-9EB45F62AC5F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{6971B438-61ED-484A-80EF-5679B73FC3FC}" srcId="{C762D9DC-C267-9446-B1CC-A95E3114C015}" destId="{B0BC72F6-8193-FD42-B124-F6D52726A515}" srcOrd="1" destOrd="0" parTransId="{43DE405C-0005-D145-AF97-5263D0BFD64F}" sibTransId="{964AE831-BB9B-824D-B098-00C54191CDE1}"/>
+    <dgm:cxn modelId="{16446A85-F567-714F-B193-7269C7206976}" type="presOf" srcId="{3E620EDA-5ADD-CC44-8C95-9FC1DF254361}" destId="{BBEAC981-0AA3-BE43-933A-96CDBD00C9A2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{A86F7C2F-8E8B-F447-B3C9-D5B16DBEC23A}" type="presOf" srcId="{DA49E6E9-CDF9-794C-AEAB-4FBD68A57F1A}" destId="{968DCEBD-CF0C-D74A-A666-31158F65E182}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{CE9B5E61-22A5-5947-B500-4861B5D405AB}" type="presOf" srcId="{66816B50-209E-8A44-99FF-FCA0FE6010CF}" destId="{1AEC4C7F-8B5D-9C4A-A0BA-DF9BE251EB21}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{0ED7FC44-A3B3-BC47-B9C7-A9AA9E2D9208}" type="presOf" srcId="{6DC6F20A-841D-E944-B9FD-E1D140F60C2C}" destId="{DFF22F0D-7EB3-DB46-B99E-239BB764C2DC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{6F34BD84-0121-8D4F-B35E-C8917B852FF4}" type="presOf" srcId="{C21A12D2-AB62-2C43-BA4D-09A91CAB6E7F}" destId="{085C6D68-61FF-5147-81E0-9AEF37B2ECCB}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{55F7D4BA-DF7D-C340-928E-78667EE5E35D}" srcId="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}" destId="{9DF1FBC3-19A9-8348-954D-040117F5C5B6}" srcOrd="0" destOrd="0" parTransId="{898657C8-0B6D-224B-8CFB-19156D73C9DA}" sibTransId="{F3CFF7FD-EA15-174D-8D76-B75F4384A783}"/>
+    <dgm:cxn modelId="{ECDBF1F1-8DB1-2F47-9295-10560BC26492}" type="presOf" srcId="{F7A43531-C46D-B547-B844-4520542846DA}" destId="{5A6C940B-8E0D-2541-B4EE-37D9893DC81C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{98EC3ADC-3C44-A241-A2BA-757D5051620F}" srcId="{6C230476-3D0D-474F-94E9-0E58DDAF8AF5}" destId="{3D5AE65B-9194-A04D-98AC-695DC8D2BA16}" srcOrd="0" destOrd="0" parTransId="{510299DD-46A5-AD46-B5A3-222A2EBA43D4}" sibTransId="{62262623-F525-B744-92D2-D50727F4632C}"/>
+    <dgm:cxn modelId="{F04AA65A-0A72-F043-9AAA-B28246B253AA}" type="presOf" srcId="{BE5B9591-AC80-4946-8C78-D7570297C39E}" destId="{11AB213E-7F90-F141-9549-20DEA56EEBBD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{E617FDFD-CC47-1A44-A1B7-1B45102440FA}" srcId="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" destId="{A8AC0743-8DDE-2742-BA27-AC8B8ED11478}" srcOrd="2" destOrd="0" parTransId="{DA49E6E9-CDF9-794C-AEAB-4FBD68A57F1A}" sibTransId="{394C33FE-BE2B-D14A-8186-87EE83BC2A29}"/>
+    <dgm:cxn modelId="{84A00250-9BE7-5348-9D7C-94A4237C2D2D}" type="presOf" srcId="{BC4BC998-E1F0-5B45-A719-663711F9FB23}" destId="{9214EDCC-7637-FA4F-A663-9416C90A1781}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{FB0EE346-51CC-5E4E-B766-63DAD646615F}" srcId="{C762D9DC-C267-9446-B1CC-A95E3114C015}" destId="{DA4300B2-2331-2046-ABC1-100C122A715A}" srcOrd="0" destOrd="0" parTransId="{41576158-B990-5740-AFD7-A7F30A9E11F8}" sibTransId="{ADB60117-51CE-ED4A-B44F-4D726CCCA9F0}"/>
+    <dgm:cxn modelId="{777DB90A-D782-314C-A7DC-BD23AEFBDC01}" type="presOf" srcId="{300BDE9E-F0C8-E145-A198-C90D0EF8BD49}" destId="{6089D488-F8D0-3F43-80B5-219C7DCFB589}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{37DA1435-D86B-5F4B-8222-1B6D9CC282BF}" type="presOf" srcId="{BC4BC998-E1F0-5B45-A719-663711F9FB23}" destId="{884F4C54-6432-7B49-A9D9-4EA1E6971C11}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{F5B46F9A-1130-754B-9BA0-4ECEE54DCA3F}" srcId="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" destId="{8F5969EE-F8BE-0348-8A1D-523AF7ADC449}" srcOrd="2" destOrd="0" parTransId="{63E4C9E5-BCE9-274B-B154-D1722539B787}" sibTransId="{E3513C9E-5BDC-2240-B7BD-13189C1D84DE}"/>
+    <dgm:cxn modelId="{F8A6846C-88D3-7B47-BAE6-5B53400B052A}" srcId="{EB608E93-0479-2148-BCC1-5BA22B50A826}" destId="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}" srcOrd="1" destOrd="0" parTransId="{0FCF08F7-3C86-6A4A-965A-08D4C71F2C83}" sibTransId="{D1378631-974B-014B-9E4C-B5B3942D43FD}"/>
+    <dgm:cxn modelId="{78A8A275-A45C-2448-ACA9-0DC72EBBDE6E}" type="presOf" srcId="{43DE405C-0005-D145-AF97-5263D0BFD64F}" destId="{25F721B1-6D69-F140-A42C-4801B2DBF60A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{1C0DD32B-51EA-7340-BAD4-366DF052646A}" type="presOf" srcId="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}" destId="{8DA6C1C2-E0BE-DE44-8DDE-6C55EBB1BE40}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{09AC1DA6-D0A3-C24C-9131-4B15F003EC87}" type="presOf" srcId="{6ECFB139-B56B-7E4E-BF1F-7CC77B2204F1}" destId="{B0B31E67-0F2F-244A-B75D-8DB3A26F446A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{9E00C10D-6030-8A4C-ACC1-B5DC4F18F09A}" type="presOf" srcId="{DA49E6E9-CDF9-794C-AEAB-4FBD68A57F1A}" destId="{199187A2-043D-8540-A3D5-F92622E95501}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{B9C3D26C-89DB-D341-9667-07933131C239}" type="presOf" srcId="{41576158-B990-5740-AFD7-A7F30A9E11F8}" destId="{59900680-E755-2F4D-8CBF-262A200A8D9D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{F3B1B910-AE71-DC43-B80F-63089CBE12C9}" type="presOf" srcId="{5E402F45-6CF9-7D49-9393-47131AFD7CE6}" destId="{0963A656-C5DC-AB41-8DEE-D65A14EA566F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{B9F31F1C-6DD2-DB47-B6EC-C72818C0D15D}" type="presOf" srcId="{43DE405C-0005-D145-AF97-5263D0BFD64F}" destId="{3977402A-F54C-7B4F-97CE-88E597C91DA3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{A0B591C8-1181-A84C-AA49-A19911497FC6}" srcId="{652DE9CE-379E-5542-8267-C153E850CFF5}" destId="{6DC6F20A-841D-E944-B9FD-E1D140F60C2C}" srcOrd="0" destOrd="0" parTransId="{F97D5CCC-FB1C-BD4D-8FC0-8444F262955E}" sibTransId="{20099B97-FDBD-6248-9B06-7F3AE556C86C}"/>
+    <dgm:cxn modelId="{CE012BDC-288E-2F4B-85E0-D9B7E794B1A9}" type="presOf" srcId="{EB608E93-0479-2148-BCC1-5BA22B50A826}" destId="{53EE5430-A405-0C45-8C3D-56B9B7B4C5EE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{1CE4048F-8B9B-D744-87BD-11459185DF44}" srcId="{B0BC72F6-8193-FD42-B124-F6D52726A515}" destId="{58A735CD-359C-954E-AB8F-0259B5D1CCE7}" srcOrd="0" destOrd="0" parTransId="{C21A12D2-AB62-2C43-BA4D-09A91CAB6E7F}" sibTransId="{3FA38BF8-2C9E-4240-8F31-7D9C338673F2}"/>
     <dgm:cxn modelId="{6D24E5BA-474E-B54A-B508-AE5A6600E646}" type="presOf" srcId="{DC9CCC13-49B8-F64C-B46E-A357D3F309D5}" destId="{DC59D9E9-9066-744D-ABF3-DD21BDB11BAD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{894FAB9C-376D-744F-A028-9D417D5EC8DD}" type="presOf" srcId="{14BF84F4-E713-F349-BD2A-D68DD017694A}" destId="{CB5AFF4C-0CEC-F643-96B6-DAC4ED874BEC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{6EB95C5C-B571-5240-8E3D-EDAD12FCAFE3}" type="presOf" srcId="{898D5F8F-CA92-7B4D-9D96-13C7CC8EB24F}" destId="{A608BD11-03C6-9149-9A0C-9460A3FE91FB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{F5B46F9A-1130-754B-9BA0-4ECEE54DCA3F}" srcId="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" destId="{8F5969EE-F8BE-0348-8A1D-523AF7ADC449}" srcOrd="2" destOrd="0" parTransId="{63E4C9E5-BCE9-274B-B154-D1722539B787}" sibTransId="{E3513C9E-5BDC-2240-B7BD-13189C1D84DE}"/>
-    <dgm:cxn modelId="{782DD2D0-5D5C-0F43-9983-36421DC4FA94}" type="presOf" srcId="{3D9D5180-F8A4-1241-9004-FDBC86CE8EB7}" destId="{022121AF-B706-D246-99BA-880E7AB5B05A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{0B26826A-375D-AC47-A747-EF197FCFC3DA}" type="presOf" srcId="{8F42AAD0-AA72-224D-89F6-60847A76B1D5}" destId="{C1AA1D1D-23B3-5348-98C0-620CC9C417E7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{2DA17B3E-21EE-964C-969D-3D2CF2623715}" srcId="{7E92DBF9-0282-3B4B-9193-15656C09A041}" destId="{4EFBB3C4-F314-AA40-AA6F-6D4A76AA74FE}" srcOrd="0" destOrd="0" parTransId="{518D05D7-25EC-904D-AC1F-588DEE03B23D}" sibTransId="{7B51DE5B-F28F-1E43-A96A-418E2C1195DE}"/>
-    <dgm:cxn modelId="{7B6DC8CC-26FA-7A40-BD86-B1BD62DED8AA}" type="presOf" srcId="{36BBC7EB-D363-3B48-8496-AA60D47185CD}" destId="{E51D9155-7752-9D41-957A-949CC75EB761}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{8D556AFB-ACA5-3343-A108-43E4822246B8}" type="presOf" srcId="{0FCF08F7-3C86-6A4A-965A-08D4C71F2C83}" destId="{48799966-5966-574A-BC3A-266F4C6BAF17}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{B88C949E-BE70-6646-B154-E56E02AA7AD8}" type="presOf" srcId="{3F5EFC20-7888-8B4C-A3B9-D9A3746FD5D9}" destId="{61A4E688-2EE9-2949-9B58-3693E86C97FB}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{346F7828-2E3C-B24C-935D-47E72C69DA19}" type="presOf" srcId="{0749699B-B7C4-6140-B4CB-8D60FBCE1ECB}" destId="{7FC46335-8ED1-2E49-A7BE-E54D41297FCD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{F081B073-88FE-7A4B-ACC7-EF443E1B1B14}" srcId="{C762D9DC-C267-9446-B1CC-A95E3114C015}" destId="{3E620EDA-5ADD-CC44-8C95-9FC1DF254361}" srcOrd="3" destOrd="0" parTransId="{2E18F920-A737-724D-B818-02F6FE67E8FC}" sibTransId="{20F03020-DD6C-8D40-A3F0-3669680E55C0}"/>
+    <dgm:cxn modelId="{D9300F27-E291-B04B-9027-512380E3CE0D}" type="presOf" srcId="{48D60804-A609-D344-B265-30D430B4E428}" destId="{78144F12-25BE-F943-8DB8-4D280CF8337F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{79A2E658-8CCD-714A-B4CA-D4E0B83709FD}" srcId="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}" destId="{9756178B-0C1F-AA4C-B73B-5C8C2B47A9E1}" srcOrd="0" destOrd="0" parTransId="{48D60804-A609-D344-B265-30D430B4E428}" sibTransId="{ACAB27F0-DFF3-9841-8916-9A4114AC1D2C}"/>
+    <dgm:cxn modelId="{8E9D1BF7-A767-874B-B492-86CEDAABA2F7}" type="presOf" srcId="{F97D5CCC-FB1C-BD4D-8FC0-8444F262955E}" destId="{56D4E8B8-277E-6C4C-B5C0-2B77C4634751}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{FFFF8D82-45AE-D14B-B967-66D253502CE8}" type="presOf" srcId="{2E18F920-A737-724D-B818-02F6FE67E8FC}" destId="{6B763081-220F-944D-96A7-37B055955D48}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{12401A03-E69F-E14E-9EC7-D65837C88D4D}" type="presOf" srcId="{DC9CCC13-49B8-F64C-B46E-A357D3F309D5}" destId="{6880828A-3410-E644-A3C4-2294177CC41C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{C9977DD5-928A-7B44-9378-13C38F8DF9C6}" type="presOf" srcId="{41576158-B990-5740-AFD7-A7F30A9E11F8}" destId="{5DFE3D87-3E56-EE42-9E29-FC62E4F1FBAE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{D437F9C1-C34A-A648-B76B-45824AC4EE74}" type="presOf" srcId="{9DF1FBC3-19A9-8348-954D-040117F5C5B6}" destId="{8B5EE93D-B5D5-D545-9E38-B095AB10F5BE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{E93D566C-95CB-ED4C-A967-373AA1778679}" type="presOf" srcId="{D98F1744-A7D7-C14A-B6A1-DD15D46D8107}" destId="{0458EB9C-8D95-A54A-BBFE-4EB0E4F471AD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{C5771104-97C6-274D-8966-AF0A7F14BF8D}" type="presOf" srcId="{B5D4559E-723E-D842-BB45-358E2F203970}" destId="{36D788C9-8DB5-D74D-BDE6-649BA5A5D5B8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{F65D7D57-E24D-CC48-B93B-C2FD8E70777C}" type="presOf" srcId="{9756178B-0C1F-AA4C-B73B-5C8C2B47A9E1}" destId="{EC0EB3A7-6AD7-5242-97AF-E79A69522BAB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{93E4E20A-FA25-5A4F-B2E2-28BA8116D850}" type="presOf" srcId="{6ECFB139-B56B-7E4E-BF1F-7CC77B2204F1}" destId="{F07A7E6F-36EA-9743-8C2B-402848A63CFF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{52253661-9A44-D34C-B6D6-78F8690EE4D6}" type="presOf" srcId="{0B970462-F13C-4D48-A4B7-10C043EEEE2B}" destId="{080C10A4-0453-4948-B1F3-2DFE4B8C8CE4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{59A8210E-2C68-1C4D-B6EE-BC38A12114EC}" type="presOf" srcId="{05B6BD45-2167-C941-A792-94ACB32DB4EC}" destId="{3E1A4BA4-A92F-724C-AE87-430A70601B53}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{1CE4048F-8B9B-D744-87BD-11459185DF44}" srcId="{B0BC72F6-8193-FD42-B124-F6D52726A515}" destId="{58A735CD-359C-954E-AB8F-0259B5D1CCE7}" srcOrd="0" destOrd="0" parTransId="{C21A12D2-AB62-2C43-BA4D-09A91CAB6E7F}" sibTransId="{3FA38BF8-2C9E-4240-8F31-7D9C338673F2}"/>
-    <dgm:cxn modelId="{28FD05AD-72D6-3342-B0A7-A596896C8656}" type="presOf" srcId="{14BF84F4-E713-F349-BD2A-D68DD017694A}" destId="{BCF273FF-CB93-044A-911C-F34C18ABCD3F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{E93D566C-95CB-ED4C-A967-373AA1778679}" type="presOf" srcId="{D98F1744-A7D7-C14A-B6A1-DD15D46D8107}" destId="{0458EB9C-8D95-A54A-BBFE-4EB0E4F471AD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{98E934AA-ECF6-7241-A5BD-70E64D2B430F}" type="presOf" srcId="{D98F1744-A7D7-C14A-B6A1-DD15D46D8107}" destId="{2060447F-F68C-B74F-BF84-BB6A544B165A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{6C76ECBB-B305-4545-B5DC-EE1511BF27C7}" type="presOf" srcId="{A3EE15A6-3F32-E047-A7C8-658B5B9A2426}" destId="{7DED3A20-7857-564A-9D1E-9551D5E2DF6D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{996FEFC3-CA7D-8344-A78E-55086C732635}" type="presOf" srcId="{43DE405C-0005-D145-AF97-5263D0BFD64F}" destId="{25F721B1-6D69-F140-A42C-4801B2DBF60A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{C3E4661B-F7DC-A54E-9FEA-034A2CC58D10}" type="presOf" srcId="{4EFBB3C4-F314-AA40-AA6F-6D4A76AA74FE}" destId="{64CE6CC6-6955-1F47-A64D-5C4536E66E8E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{84A00250-9BE7-5348-9D7C-94A4237C2D2D}" type="presOf" srcId="{BC4BC998-E1F0-5B45-A719-663711F9FB23}" destId="{9214EDCC-7637-FA4F-A663-9416C90A1781}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{645DC926-9A47-944A-98CE-98FC66596F96}" type="presOf" srcId="{E1246F00-5110-6146-85B3-F18EAD31DE44}" destId="{96296898-BE98-0247-83BE-61F5D3D682F5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{7DB2C1AF-3B5B-7C43-854C-BF3A2DB639BA}" srcId="{3D5AE65B-9194-A04D-98AC-695DC8D2BA16}" destId="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" srcOrd="0" destOrd="0" parTransId="{66816B50-209E-8A44-99FF-FCA0FE6010CF}" sibTransId="{003A5410-B948-1B4C-AECA-2D523EED1A72}"/>
-    <dgm:cxn modelId="{D437F9C1-C34A-A648-B76B-45824AC4EE74}" type="presOf" srcId="{9DF1FBC3-19A9-8348-954D-040117F5C5B6}" destId="{8B5EE93D-B5D5-D545-9E38-B095AB10F5BE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{1C512F6D-FBAA-3B49-B60D-E5DFB50B2A87}" type="presOf" srcId="{6C230476-3D0D-474F-94E9-0E58DDAF8AF5}" destId="{E462CEA6-69E8-2346-9B02-3EDF954B7021}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{751DFE1C-CFA6-BB4D-9A10-F5723CA5A01D}" type="presOf" srcId="{898657C8-0B6D-224B-8CFB-19156D73C9DA}" destId="{8E9E86BF-4214-C04F-819A-80928C1A4988}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{CE012BDC-288E-2F4B-85E0-D9B7E794B1A9}" type="presOf" srcId="{EB608E93-0479-2148-BCC1-5BA22B50A826}" destId="{53EE5430-A405-0C45-8C3D-56B9B7B4C5EE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{5C815C7F-6EED-F340-8731-E7461FCCF51C}" type="presOf" srcId="{C21A12D2-AB62-2C43-BA4D-09A91CAB6E7F}" destId="{CD750812-B108-564F-992D-C437D68E95A1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{8F1C49EE-1DF5-AE4D-9F7A-408782E8D8FD}" type="presOf" srcId="{63E4C9E5-BCE9-274B-B154-D1722539B787}" destId="{EC1947AE-4E19-6545-8360-1E46FEF87CE8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{777DB90A-D782-314C-A7DC-BD23AEFBDC01}" type="presOf" srcId="{300BDE9E-F0C8-E145-A198-C90D0EF8BD49}" destId="{6089D488-F8D0-3F43-80B5-219C7DCFB589}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{3348C0B5-1D0A-6E45-891C-EA5721A2DED7}" type="presOf" srcId="{0749699B-B7C4-6140-B4CB-8D60FBCE1ECB}" destId="{36C0C19B-3F9B-2049-BB73-D3B74079B1BA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{208AF81C-E7E9-5E47-916E-277546BC2951}" type="presOf" srcId="{DE6250AC-E2C3-EA4C-90F4-F144D5C45412}" destId="{1A86F6FD-7823-CA48-AB5A-F31345841067}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{1C0DD32B-51EA-7340-BAD4-366DF052646A}" type="presOf" srcId="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}" destId="{8DA6C1C2-E0BE-DE44-8DDE-6C55EBB1BE40}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{6EBC92F6-8833-CF4E-BBC0-9E0071879B33}" type="presOf" srcId="{94300211-45FB-9547-B995-E1E57425CDE7}" destId="{9FDC99B0-D551-004A-864C-6DCAFEB88B76}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{57B49347-DDE9-3943-BD16-CE8F3969BDEF}" type="presOf" srcId="{48D60804-A609-D344-B265-30D430B4E428}" destId="{2B0D2414-9C87-0445-8FBF-CB229BF7118E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{ECDBF1F1-8DB1-2F47-9295-10560BC26492}" type="presOf" srcId="{F7A43531-C46D-B547-B844-4520542846DA}" destId="{5A6C940B-8E0D-2541-B4EE-37D9893DC81C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{507C37D9-DF70-C049-AB45-6D6194C6EDD1}" srcId="{3D5AE65B-9194-A04D-98AC-695DC8D2BA16}" destId="{EB608E93-0479-2148-BCC1-5BA22B50A826}" srcOrd="2" destOrd="0" parTransId="{DE6250AC-E2C3-EA4C-90F4-F144D5C45412}" sibTransId="{873FE768-EBDB-5444-A928-15F6A44CCEAB}"/>
-    <dgm:cxn modelId="{75F0B2F8-DA7D-6F4C-9970-2C891AE0C933}" type="presOf" srcId="{4FDA31E9-0995-E646-B247-48C734F29F55}" destId="{96B1CDE0-C35A-CB43-9A64-AE7BDFB44B3E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{7BDF0CB4-4494-3841-A0C2-B96746C922B8}" srcId="{EB608E93-0479-2148-BCC1-5BA22B50A826}" destId="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}" srcOrd="0" destOrd="0" parTransId="{8F42AAD0-AA72-224D-89F6-60847A76B1D5}" sibTransId="{C3BA1502-7EEB-0B4D-89AF-D304786068A6}"/>
-    <dgm:cxn modelId="{1D5BC62B-2A2D-3D4B-BFBC-1F8D84208103}" srcId="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" destId="{7E92DBF9-0282-3B4B-9193-15656C09A041}" srcOrd="3" destOrd="0" parTransId="{84C2140E-F94B-3A42-9984-32D5D0D67690}" sibTransId="{030D0447-EF41-D64C-8E70-01DF93EB72FB}"/>
-    <dgm:cxn modelId="{E952C6BB-929E-ED4F-90DC-A4D3740B3FF3}" type="presOf" srcId="{84C2140E-F94B-3A42-9984-32D5D0D67690}" destId="{EAE6DA3D-6DCE-8B43-86D6-453237F6F64F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{1F843B3F-7DC5-414A-9B4E-30DCB65002A0}" srcId="{2064DC40-2F6A-7246-96EB-B7DCB07874C8}" destId="{94300211-45FB-9547-B995-E1E57425CDE7}" srcOrd="0" destOrd="0" parTransId="{4FDA31E9-0995-E646-B247-48C734F29F55}" sibTransId="{CCCEAC01-3AAB-0740-B4DD-8DC6B0962AE7}"/>
-    <dgm:cxn modelId="{56D695B1-E3AA-3541-85E2-CB6032787A20}" srcId="{A8AC0743-8DDE-2742-BA27-AC8B8ED11478}" destId="{C6790FB4-8208-8143-B098-50B34734D56A}" srcOrd="0" destOrd="0" parTransId="{3D9D5180-F8A4-1241-9004-FDBC86CE8EB7}" sibTransId="{9684E716-804F-5841-98EA-1142E391B6CA}"/>
+    <dgm:cxn modelId="{1200454C-9EF6-0748-9DA5-378488D8353D}" srcId="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" destId="{CBD00C11-7705-4B46-A507-504E11D7B2C4}" srcOrd="0" destOrd="0" parTransId="{6ECFB139-B56B-7E4E-BF1F-7CC77B2204F1}" sibTransId="{F18EA58F-3780-2344-B441-40FB946DF195}"/>
+    <dgm:cxn modelId="{6B7ADC54-81D4-B842-8BAA-89D852EF023D}" type="presOf" srcId="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}" destId="{8F0E1068-96D7-094C-A746-F91F87169C20}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{6B677ED3-2EE9-3248-A2FB-E4811A876FBA}" type="presOf" srcId="{3F5EFC20-7888-8B4C-A3B9-D9A3746FD5D9}" destId="{9F3C9693-87FA-7F45-B58A-F884460F249C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{9E00C10D-6030-8A4C-ACC1-B5DC4F18F09A}" type="presOf" srcId="{DA49E6E9-CDF9-794C-AEAB-4FBD68A57F1A}" destId="{199187A2-043D-8540-A3D5-F92622E95501}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{98EC3ADC-3C44-A241-A2BA-757D5051620F}" srcId="{6C230476-3D0D-474F-94E9-0E58DDAF8AF5}" destId="{3D5AE65B-9194-A04D-98AC-695DC8D2BA16}" srcOrd="0" destOrd="0" parTransId="{510299DD-46A5-AD46-B5A3-222A2EBA43D4}" sibTransId="{62262623-F525-B744-92D2-D50727F4632C}"/>
-    <dgm:cxn modelId="{A88E5FD2-A613-7B4D-B5C5-FADE7864F541}" type="presOf" srcId="{66816B50-209E-8A44-99FF-FCA0FE6010CF}" destId="{2680328F-7469-384B-A713-47DAA1730724}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{F8A6846C-88D3-7B47-BAE6-5B53400B052A}" srcId="{EB608E93-0479-2148-BCC1-5BA22B50A826}" destId="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}" srcOrd="1" destOrd="0" parTransId="{0FCF08F7-3C86-6A4A-965A-08D4C71F2C83}" sibTransId="{D1378631-974B-014B-9E4C-B5B3942D43FD}"/>
-    <dgm:cxn modelId="{25175D81-E26B-6A4B-997A-5F057943061D}" type="presOf" srcId="{B0BC72F6-8193-FD42-B124-F6D52726A515}" destId="{84D18324-7849-AF4F-A07E-80E004C8B650}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{1200454C-9EF6-0748-9DA5-378488D8353D}" srcId="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" destId="{CBD00C11-7705-4B46-A507-504E11D7B2C4}" srcOrd="0" destOrd="0" parTransId="{6ECFB139-B56B-7E4E-BF1F-7CC77B2204F1}" sibTransId="{F18EA58F-3780-2344-B441-40FB946DF195}"/>
-    <dgm:cxn modelId="{A86F7C2F-8E8B-F447-B3C9-D5B16DBEC23A}" type="presOf" srcId="{DA49E6E9-CDF9-794C-AEAB-4FBD68A57F1A}" destId="{968DCEBD-CF0C-D74A-A666-31158F65E182}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{98306D63-FFBF-4B41-847D-6CAC1EA77F57}" srcId="{CBD00C11-7705-4B46-A507-504E11D7B2C4}" destId="{05B6BD45-2167-C941-A792-94ACB32DB4EC}" srcOrd="0" destOrd="0" parTransId="{D98F1744-A7D7-C14A-B6A1-DD15D46D8107}" sibTransId="{41378A21-F6F6-AC47-B392-C0CCEED89946}"/>
-    <dgm:cxn modelId="{DB1423D0-A323-1243-91E9-AC1BD456CF7F}" type="presOf" srcId="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" destId="{02E0FECA-2589-C94E-8421-1373276E6CD0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{161041FB-0B6D-7942-9675-27BD612AE577}" type="presOf" srcId="{43DE405C-0005-D145-AF97-5263D0BFD64F}" destId="{3977402A-F54C-7B4F-97CE-88E597C91DA3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{6E431DE5-A5CB-904E-AC51-9908AD548198}" srcId="{8F5969EE-F8BE-0348-8A1D-523AF7ADC449}" destId="{2F71905B-FED7-7946-BB13-3426F23C1911}" srcOrd="0" destOrd="0" parTransId="{0749699B-B7C4-6140-B4CB-8D60FBCE1ECB}" sibTransId="{DA70BC87-3097-4A43-94C7-A082FCE90909}"/>
-    <dgm:cxn modelId="{39765572-6D1C-BC4E-9CFD-035C64214606}" type="presOf" srcId="{58A735CD-359C-954E-AB8F-0259B5D1CCE7}" destId="{69AC3AD2-ED21-5344-AD1D-FDFEEE7C4C5B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{346F7828-2E3C-B24C-935D-47E72C69DA19}" type="presOf" srcId="{0749699B-B7C4-6140-B4CB-8D60FBCE1ECB}" destId="{7FC46335-8ED1-2E49-A7BE-E54D41297FCD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{E0FA02E1-0C9E-5741-B722-4FF2428F452F}" type="presOf" srcId="{B1871CE9-AA57-7E40-9F44-89545C773C31}" destId="{09A02069-0039-4049-80CB-8B6C97B26549}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{DCAEB176-E0ED-2840-9D0F-966856FBF6F5}" type="presOf" srcId="{A8AC0743-8DDE-2742-BA27-AC8B8ED11478}" destId="{2A221514-4A03-4B45-B5AF-749FB8232375}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{D9300F27-E291-B04B-9027-512380E3CE0D}" type="presOf" srcId="{48D60804-A609-D344-B265-30D430B4E428}" destId="{78144F12-25BE-F943-8DB8-4D280CF8337F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{512615FE-EEA4-3B4F-B5DE-57D9F2585BAC}" srcId="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" destId="{E1246F00-5110-6146-85B3-F18EAD31DE44}" srcOrd="4" destOrd="0" parTransId="{A3EE15A6-3F32-E047-A7C8-658B5B9A2426}" sibTransId="{12500183-1309-E045-9F84-801F4A2275FA}"/>
-    <dgm:cxn modelId="{DD6FAD2D-F789-6F4A-B4A8-DF09C8211A34}" srcId="{E1246F00-5110-6146-85B3-F18EAD31DE44}" destId="{1FCD6FA2-2EC1-E044-8817-90704567D52F}" srcOrd="0" destOrd="0" parTransId="{98BE4178-0B33-D54A-91F1-7CD2B3AC77E2}" sibTransId="{AB2C0215-39C8-5D44-ABC6-4F4701B566BF}"/>
-    <dgm:cxn modelId="{684E744E-37CF-B14E-BC3F-1EB3F048D34E}" type="presOf" srcId="{300BDE9E-F0C8-E145-A198-C90D0EF8BD49}" destId="{97838F66-388F-334E-8C48-6883CD119D60}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{9997DE30-3ADF-2E45-86FA-F99D6F17FC2E}" type="presOf" srcId="{2F71905B-FED7-7946-BB13-3426F23C1911}" destId="{743C9E64-CA35-3346-BD28-35C33D90F652}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{4DAAB8D2-AC24-EF4E-A35E-DF3DAB679966}" type="presOf" srcId="{2064DC40-2F6A-7246-96EB-B7DCB07874C8}" destId="{D90297FE-FAC7-9042-A8CC-4C7D825B33BF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{E617FDFD-CC47-1A44-A1B7-1B45102440FA}" srcId="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" destId="{A8AC0743-8DDE-2742-BA27-AC8B8ED11478}" srcOrd="2" destOrd="0" parTransId="{DA49E6E9-CDF9-794C-AEAB-4FBD68A57F1A}" sibTransId="{394C33FE-BE2B-D14A-8186-87EE83BC2A29}"/>
-    <dgm:cxn modelId="{EF22345A-BC2D-DF4E-8D95-F54CD52902C0}" type="presOf" srcId="{518D05D7-25EC-904D-AC1F-588DEE03B23D}" destId="{CC83B46B-5011-A34F-BF53-6A906E35A6D8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{A467DF2D-BC30-E045-8362-C42E60148128}" srcId="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" destId="{2064DC40-2F6A-7246-96EB-B7DCB07874C8}" srcOrd="3" destOrd="0" parTransId="{898D5F8F-CA92-7B4D-9D96-13C7CC8EB24F}" sibTransId="{DBD9B648-1F16-814B-85AA-41C3AC0F5A3F}"/>
-    <dgm:cxn modelId="{E5F81167-C364-1545-A7C5-95F0D760BF63}" srcId="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" destId="{36BBC7EB-D363-3B48-8496-AA60D47185CD}" srcOrd="0" destOrd="0" parTransId="{300BDE9E-F0C8-E145-A198-C90D0EF8BD49}" sibTransId="{47991693-D9A7-9441-8FBC-ECF07DA73E6A}"/>
-    <dgm:cxn modelId="{09AC1DA6-D0A3-C24C-9131-4B15F003EC87}" type="presOf" srcId="{6ECFB139-B56B-7E4E-BF1F-7CC77B2204F1}" destId="{B0B31E67-0F2F-244A-B75D-8DB3A26F446A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{4C26807E-41C6-BD4F-98C8-C78B73CB3A48}" srcId="{36BBC7EB-D363-3B48-8496-AA60D47185CD}" destId="{B1871CE9-AA57-7E40-9F44-89545C773C31}" srcOrd="0" destOrd="0" parTransId="{3F5EFC20-7888-8B4C-A3B9-D9A3746FD5D9}" sibTransId="{5D8571E4-D1F1-6648-B5D0-EB4F7F948761}"/>
-    <dgm:cxn modelId="{1C81621C-E44B-8C43-A258-03B24FAC54F1}" type="presOf" srcId="{30FE5FD2-03E7-C142-AA91-76709434DD90}" destId="{22159CD9-4EC1-E544-98E6-9AD9F99F03AF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{42FDA32E-A0D0-3C47-A7C4-1B51C6B7C1D8}" type="presOf" srcId="{C6790FB4-8208-8143-B098-50B34734D56A}" destId="{9F55E6EF-25E4-B542-8DEE-25656226127F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{9A1802E0-CAF2-EF4B-A49D-F3696436A418}" srcId="{30FE5FD2-03E7-C142-AA91-76709434DD90}" destId="{F7A43531-C46D-B547-B844-4520542846DA}" srcOrd="0" destOrd="0" parTransId="{14BF84F4-E713-F349-BD2A-D68DD017694A}" sibTransId="{D10E3117-503F-804D-858D-A55F25900986}"/>
-    <dgm:cxn modelId="{93E4E20A-FA25-5A4F-B2E2-28BA8116D850}" type="presOf" srcId="{6ECFB139-B56B-7E4E-BF1F-7CC77B2204F1}" destId="{F07A7E6F-36EA-9743-8C2B-402848A63CFF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{37DA1435-D86B-5F4B-8222-1B6D9CC282BF}" type="presOf" srcId="{BC4BC998-E1F0-5B45-A719-663711F9FB23}" destId="{884F4C54-6432-7B49-A9D9-4EA1E6971C11}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{AB312320-284C-6A44-ACA0-F236A55AA413}" type="presOf" srcId="{CBD00C11-7705-4B46-A507-504E11D7B2C4}" destId="{D0686948-65B5-CE4B-99C1-9EB45F62AC5F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{909E12BF-F4AD-8A4A-9DFE-5E3A5D3BC768}" type="presOf" srcId="{98BE4178-0B33-D54A-91F1-7CD2B3AC77E2}" destId="{04C15EBF-48BF-2D4C-BF9B-0823F14313EF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{97ECA95F-38BC-2F49-B680-1948140DDC40}" type="presOf" srcId="{7E92DBF9-0282-3B4B-9193-15656C09A041}" destId="{AFB00BA5-37D3-4D49-ABEF-E265A327F349}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{7D6DE11C-6A19-3A4D-BB4D-CAA7B0ABA0DA}" srcId="{1B3C97F0-1B5E-DE4B-BD53-04B0F98FD209}" destId="{30FE5FD2-03E7-C142-AA91-76709434DD90}" srcOrd="1" destOrd="0" parTransId="{DC9CCC13-49B8-F64C-B46E-A357D3F309D5}" sibTransId="{749523E1-DB0A-7740-9A56-5B4F05E26FCB}"/>
-    <dgm:cxn modelId="{6805E153-C0A4-F14B-8B2F-2FCE6F5E858B}" type="presOf" srcId="{0FCF08F7-3C86-6A4A-965A-08D4C71F2C83}" destId="{9C06130D-D3CF-6C4B-9249-8865DD724342}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{55F7D4BA-DF7D-C340-928E-78667EE5E35D}" srcId="{7C549909-39C6-634F-AD6F-5BC74E5D5A0B}" destId="{9DF1FBC3-19A9-8348-954D-040117F5C5B6}" srcOrd="0" destOrd="0" parTransId="{898657C8-0B6D-224B-8CFB-19156D73C9DA}" sibTransId="{F3CFF7FD-EA15-174D-8D76-B75F4384A783}"/>
-    <dgm:cxn modelId="{0E9A348A-EA3F-444C-BFA5-13469C10E39B}" type="presOf" srcId="{898657C8-0B6D-224B-8CFB-19156D73C9DA}" destId="{8767306D-9113-BC4B-81AA-7FB530A91291}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{3934643F-6CF9-5842-8619-19B7B97BAD26}" type="presOf" srcId="{A3EE15A6-3F32-E047-A7C8-658B5B9A2426}" destId="{49C1BB80-7116-0243-8559-F49FE35EAC8C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{473CB1A4-FFCF-A34A-9B80-740DDD576AEC}" type="presOf" srcId="{4FDA31E9-0995-E646-B247-48C734F29F55}" destId="{769BF5E9-2773-7642-A2AF-516B0418FC0F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{12401A03-E69F-E14E-9EC7-D65837C88D4D}" type="presOf" srcId="{DC9CCC13-49B8-F64C-B46E-A357D3F309D5}" destId="{6880828A-3410-E644-A3C4-2294177CC41C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{7D5B75CF-0F32-2E4A-8660-0FF6CF30448C}" type="presOf" srcId="{8F5969EE-F8BE-0348-8A1D-523AF7ADC449}" destId="{ED82EB34-8097-994C-90F2-D4621919418A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{CE9B5E61-22A5-5947-B500-4861B5D405AB}" type="presOf" srcId="{66816B50-209E-8A44-99FF-FCA0FE6010CF}" destId="{1AEC4C7F-8B5D-9C4A-A0BA-DF9BE251EB21}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{5C5CB6A2-990A-FB42-A1B8-545AEA64B2E2}" type="presOf" srcId="{C21A12D2-AB62-2C43-BA4D-09A91CAB6E7F}" destId="{085C6D68-61FF-5147-81E0-9AEF37B2ECCB}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{0586DEEA-8F0A-664D-9F37-77808E6A4FFF}" type="presOf" srcId="{1FCD6FA2-2EC1-E044-8817-90704567D52F}" destId="{98E56F84-7B9F-E448-A77F-BECF084C032C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{8ED90E71-1FD6-F14C-A7E9-AB42D57BB316}" type="presOf" srcId="{98BE4178-0B33-D54A-91F1-7CD2B3AC77E2}" destId="{C08397E8-4357-1040-B413-6547DDCD0CDD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{CE301E01-2C61-1446-ACAA-DDD710CBC21B}" type="presOf" srcId="{DE6250AC-E2C3-EA4C-90F4-F144D5C45412}" destId="{F2B8E9EC-9E8D-EF4F-8069-8CF8FD8833B2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{06FADF7B-BEC5-7C43-994B-AC10C0BB5165}" type="presOf" srcId="{3D9D5180-F8A4-1241-9004-FDBC86CE8EB7}" destId="{5DA24466-CB9E-0F43-B8A3-FA63AE383C78}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{714AF0CD-13D5-5241-9539-5CA4808D0AD3}" type="presOf" srcId="{3D5AE65B-9194-A04D-98AC-695DC8D2BA16}" destId="{61D69160-A7CD-9049-954F-FA5CBF774AED}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{F65D7D57-E24D-CC48-B93B-C2FD8E70777C}" type="presOf" srcId="{9756178B-0C1F-AA4C-B73B-5C8C2B47A9E1}" destId="{EC0EB3A7-6AD7-5242-97AF-E79A69522BAB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{7D2CB5FB-2947-6944-B2CF-3F1126D5C29C}" type="presOf" srcId="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" destId="{B895C344-133F-4340-80A0-685E27E999D6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{0726FDF0-FFFF-FF4B-B05F-97DF4549DCF5}" type="presOf" srcId="{84C2140E-F94B-3A42-9984-32D5D0D67690}" destId="{AD7BBE0F-FABE-714F-B19E-9F525577B2B5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{C2E8BEEA-6AB0-1540-BCA7-7D857D0EE50A}" type="presOf" srcId="{63E4C9E5-BCE9-274B-B154-D1722539B787}" destId="{E51D49A7-6AFC-F04F-9B53-612EDC5C173D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{6B7ADC54-81D4-B842-8BAA-89D852EF023D}" type="presOf" srcId="{8A21709E-6FE0-0845-AA28-2B8FCDAA188E}" destId="{8F0E1068-96D7-094C-A746-F91F87169C20}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{7A52DB0A-EE7E-704B-B790-A9FED4B59CD1}" type="presOf" srcId="{518D05D7-25EC-904D-AC1F-588DEE03B23D}" destId="{DA2BBBC5-96AE-D245-B903-7F481B166D03}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{6971B438-61ED-484A-80EF-5679B73FC3FC}" srcId="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" destId="{B0BC72F6-8193-FD42-B124-F6D52726A515}" srcOrd="1" destOrd="0" parTransId="{43DE405C-0005-D145-AF97-5263D0BFD64F}" sibTransId="{964AE831-BB9B-824D-B098-00C54191CDE1}"/>
-    <dgm:cxn modelId="{F200E26E-0AA3-104C-A445-0A16851EF130}" type="presOf" srcId="{8F42AAD0-AA72-224D-89F6-60847A76B1D5}" destId="{CF5C0BC9-1C55-6D44-9740-9A1957FD4485}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{844E2698-F22A-D343-AB95-197D90F2F9D0}" srcId="{3D5AE65B-9194-A04D-98AC-695DC8D2BA16}" destId="{C1B123D7-ACAF-5649-AFFC-155C51CC2222}" srcOrd="1" destOrd="0" parTransId="{BC4BC998-E1F0-5B45-A719-663711F9FB23}" sibTransId="{DDB0B02F-B0F4-F846-A7E4-E7A12917CEB3}"/>
-    <dgm:cxn modelId="{A2C74DA4-9E8F-584E-AB55-C6991E629AD8}" type="presOf" srcId="{898D5F8F-CA92-7B4D-9D96-13C7CC8EB24F}" destId="{D5068B54-DECB-5C40-8C43-3E238EA1A151}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{36D2B51A-8C23-D344-BFD7-7BDE4542C444}" type="presParOf" srcId="{E462CEA6-69E8-2346-9B02-3EDF954B7021}" destId="{C892B71B-46E3-4844-994D-39FDFFD52BCE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{B38108A3-27D1-D348-A46A-AF11C36EAA65}" type="presParOf" srcId="{C892B71B-46E3-4844-994D-39FDFFD52BCE}" destId="{61D69160-A7CD-9049-954F-FA5CBF774AED}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{045CCB90-10CE-E541-AC44-21AB5E5DD0A0}" type="presParOf" srcId="{C892B71B-46E3-4844-994D-39FDFFD52BCE}" destId="{B1B8291F-AF33-5D48-99F4-EFCEA4F477B2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
@@ -2722,16 +3135,6 @@
     <dgm:cxn modelId="{D0455C6A-4EAE-7C4F-BE18-58A48AAFCD76}" type="presParOf" srcId="{B47F0335-AD5E-0A4E-9E4A-4DCE074ACFFC}" destId="{C5780C21-D1DD-A745-8AA9-1E4DA9C5756E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{D2E8529A-5E68-534E-989C-5489EA1C2F79}" type="presParOf" srcId="{C5780C21-D1DD-A745-8AA9-1E4DA9C5756E}" destId="{743C9E64-CA35-3346-BD28-35C33D90F652}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{9AF4392A-7B71-EC49-B0D7-6A74BB742E78}" type="presParOf" srcId="{C5780C21-D1DD-A745-8AA9-1E4DA9C5756E}" destId="{817428C6-41F1-ED4A-89B3-5BDEED892E6A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{C556339F-A40C-5E49-B650-16A84ACE605E}" type="presParOf" srcId="{67D304E8-2CDA-3847-A46A-66DB2307B607}" destId="{EAE6DA3D-6DCE-8B43-86D6-453237F6F64F}" srcOrd="6" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{E6DB8DB5-BC4D-6848-8BDA-FC0DADE11942}" type="presParOf" srcId="{EAE6DA3D-6DCE-8B43-86D6-453237F6F64F}" destId="{AD7BBE0F-FABE-714F-B19E-9F525577B2B5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{1601DDBE-6124-3947-818D-95173BCBD30C}" type="presParOf" srcId="{67D304E8-2CDA-3847-A46A-66DB2307B607}" destId="{F5455EA7-4F95-6E44-B4DD-7E31D6C976CF}" srcOrd="7" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{38C422C8-EBCD-774A-897D-3636770E12D3}" type="presParOf" srcId="{F5455EA7-4F95-6E44-B4DD-7E31D6C976CF}" destId="{AFB00BA5-37D3-4D49-ABEF-E265A327F349}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{0287E863-CE30-8A4A-B7E9-17B33A7A1F84}" type="presParOf" srcId="{F5455EA7-4F95-6E44-B4DD-7E31D6C976CF}" destId="{BE95D251-3395-B24E-8B8F-DEEE14D3DB84}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{AAA667A0-B3B5-124F-954B-B211B52D7288}" type="presParOf" srcId="{BE95D251-3395-B24E-8B8F-DEEE14D3DB84}" destId="{DA2BBBC5-96AE-D245-B903-7F481B166D03}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{F86BAE4E-740A-E445-A17D-C8D1126BEEB7}" type="presParOf" srcId="{DA2BBBC5-96AE-D245-B903-7F481B166D03}" destId="{CC83B46B-5011-A34F-BF53-6A906E35A6D8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{9DE47A37-3D40-3041-8B1F-AA5D2283D90E}" type="presParOf" srcId="{BE95D251-3395-B24E-8B8F-DEEE14D3DB84}" destId="{41391B8F-AC13-DF4C-97EE-0D164D665333}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{81C1ECC8-65D6-F049-BC25-C297CB09CFBE}" type="presParOf" srcId="{41391B8F-AC13-DF4C-97EE-0D164D665333}" destId="{64CE6CC6-6955-1F47-A64D-5C4536E66E8E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{04301BA3-5B1C-2A4E-8BB9-A00BDFB6352E}" type="presParOf" srcId="{41391B8F-AC13-DF4C-97EE-0D164D665333}" destId="{54B0ACB6-DE3A-0945-B9E2-CC9D398D1FC9}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{58792A76-0EB1-4647-8820-BA018A57448A}" type="presParOf" srcId="{B1B8291F-AF33-5D48-99F4-EFCEA4F477B2}" destId="{9214EDCC-7637-FA4F-A663-9416C90A1781}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{DA2D0538-A725-B14B-B089-F455A2AE4AC3}" type="presParOf" srcId="{9214EDCC-7637-FA4F-A663-9416C90A1781}" destId="{884F4C54-6432-7B49-A9D9-4EA1E6971C11}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{F92A511A-F715-9E4A-A86D-8AFC6C810DBA}" type="presParOf" srcId="{B1B8291F-AF33-5D48-99F4-EFCEA4F477B2}" destId="{B996FCDD-2B3D-5E4F-BE3F-3B9749B49997}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
@@ -2747,16 +3150,41 @@
     <dgm:cxn modelId="{06F84616-6B70-3B4C-87DA-885155497593}" type="presParOf" srcId="{7B01EE8E-0002-8644-B406-145BE45E0878}" destId="{3B569781-F5BD-5E40-B302-18DD6386FFFB}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{9A7FB4C6-D675-D04F-86C9-F2C1BB4C7FBE}" type="presParOf" srcId="{3B569781-F5BD-5E40-B302-18DD6386FFFB}" destId="{3E1A4BA4-A92F-724C-AE87-430A70601B53}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{0130176B-B678-884F-9443-E9632D839B27}" type="presParOf" srcId="{3B569781-F5BD-5E40-B302-18DD6386FFFB}" destId="{0FCCF158-7203-874A-BC78-6D0864195E77}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{D315A0C1-A558-984C-9088-1F38C510AE1C}" type="presParOf" srcId="{598F85C8-C84D-C143-8558-EE261698AAD1}" destId="{25F721B1-6D69-F140-A42C-4801B2DBF60A}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{19484952-19BF-374B-A85E-5162086DD3A7}" type="presParOf" srcId="{25F721B1-6D69-F140-A42C-4801B2DBF60A}" destId="{3977402A-F54C-7B4F-97CE-88E597C91DA3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{68BA6CCC-DBD9-BE4F-8D63-4BCFD9DEDBE4}" type="presParOf" srcId="{598F85C8-C84D-C143-8558-EE261698AAD1}" destId="{392EE4AA-6742-B242-BEC9-4763AF49A400}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{C4DA641D-9CD2-B642-B714-781CD9231D63}" type="presParOf" srcId="{392EE4AA-6742-B242-BEC9-4763AF49A400}" destId="{84D18324-7849-AF4F-A07E-80E004C8B650}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{6225BB4B-0B19-524F-8C4B-804440F3BF1D}" type="presParOf" srcId="{392EE4AA-6742-B242-BEC9-4763AF49A400}" destId="{1D3F560C-301B-434B-A1FD-2D4533B00084}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{A89A951A-1990-F441-BAC4-6F4D6E91C802}" type="presParOf" srcId="{1D3F560C-301B-434B-A1FD-2D4533B00084}" destId="{CD750812-B108-564F-992D-C437D68E95A1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{431A3447-0A6B-7A40-B57A-49FBCC2BFFF5}" type="presParOf" srcId="{CD750812-B108-564F-992D-C437D68E95A1}" destId="{085C6D68-61FF-5147-81E0-9AEF37B2ECCB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{A914C868-C605-F543-81B1-FFD2916C1AE3}" type="presParOf" srcId="{1D3F560C-301B-434B-A1FD-2D4533B00084}" destId="{AE3ABCE3-88A7-4D40-8B8A-323DD095ABDD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{DCE443D6-C0A7-D640-9409-B09F841530EB}" type="presParOf" srcId="{AE3ABCE3-88A7-4D40-8B8A-323DD095ABDD}" destId="{69AC3AD2-ED21-5344-AD1D-FDFEEE7C4C5B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{1A594379-2FF4-F24A-9791-A0E9B1754962}" type="presParOf" srcId="{AE3ABCE3-88A7-4D40-8B8A-323DD095ABDD}" destId="{4213F435-3482-8244-A9A1-055C2931906F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{CAE19902-C176-3A4C-8707-E9A4C332AD6E}" type="presParOf" srcId="{598F85C8-C84D-C143-8558-EE261698AAD1}" destId="{36D788C9-8DB5-D74D-BDE6-649BA5A5D5B8}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{7EBA79EB-7E61-0443-BD31-5A131425D5E9}" type="presParOf" srcId="{36D788C9-8DB5-D74D-BDE6-649BA5A5D5B8}" destId="{D4F4059E-9072-DD44-9070-1FDB3E4A368D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{34B57D73-C3DA-A142-B97B-741CA92E6813}" type="presParOf" srcId="{598F85C8-C84D-C143-8558-EE261698AAD1}" destId="{C1382441-915F-C04A-9929-FBEA1CF2BD36}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{FE7D2BAE-897B-DA48-B860-1933E6F6C13F}" type="presParOf" srcId="{C1382441-915F-C04A-9929-FBEA1CF2BD36}" destId="{C6AA8951-971D-8D46-A6B7-A3287247CC64}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{33C9021A-8588-B843-827B-EDBAB5471FC7}" type="presParOf" srcId="{C1382441-915F-C04A-9929-FBEA1CF2BD36}" destId="{DEA98603-1475-6643-B90D-B4C5B3BB2727}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{F2130C78-E568-DF47-AB29-A9319385756F}" type="presParOf" srcId="{DEA98603-1475-6643-B90D-B4C5B3BB2727}" destId="{5DFE3D87-3E56-EE42-9E29-FC62E4F1FBAE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{B2513842-29B5-154E-AA7B-EF20367EA931}" type="presParOf" srcId="{5DFE3D87-3E56-EE42-9E29-FC62E4F1FBAE}" destId="{59900680-E755-2F4D-8CBF-262A200A8D9D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{04869C4C-55C2-5E40-9621-7CE3FA587847}" type="presParOf" srcId="{DEA98603-1475-6643-B90D-B4C5B3BB2727}" destId="{5A3C6DA5-EB5E-6B46-BC3A-243E7E9C2D82}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{B01F141F-5DC9-9B4B-AA46-CA8C2D8ECE70}" type="presParOf" srcId="{5A3C6DA5-EB5E-6B46-BC3A-243E7E9C2D82}" destId="{8A60DE61-E72C-854C-836C-D906D1A70AB7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{A35ECF73-B925-6B40-B81B-C2E9277D3902}" type="presParOf" srcId="{5A3C6DA5-EB5E-6B46-BC3A-243E7E9C2D82}" destId="{8EF72282-BF11-7743-901F-6D51777AFDF4}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{8C2DFF58-3AF6-3B43-AAC1-C10BFC355C03}" type="presParOf" srcId="{DEA98603-1475-6643-B90D-B4C5B3BB2727}" destId="{25F721B1-6D69-F140-A42C-4801B2DBF60A}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{38724C78-15EF-D34B-B14C-A011D910E1AA}" type="presParOf" srcId="{25F721B1-6D69-F140-A42C-4801B2DBF60A}" destId="{3977402A-F54C-7B4F-97CE-88E597C91DA3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{345C3137-675E-C44C-B995-7B8350595F71}" type="presParOf" srcId="{DEA98603-1475-6643-B90D-B4C5B3BB2727}" destId="{392EE4AA-6742-B242-BEC9-4763AF49A400}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{4CA3DA70-5FDA-624D-B25A-D60FA1DCFFB4}" type="presParOf" srcId="{392EE4AA-6742-B242-BEC9-4763AF49A400}" destId="{84D18324-7849-AF4F-A07E-80E004C8B650}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{F8D921A7-F29C-1F4C-8EB4-435E4CBBF994}" type="presParOf" srcId="{392EE4AA-6742-B242-BEC9-4763AF49A400}" destId="{1D3F560C-301B-434B-A1FD-2D4533B00084}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{A80807D7-D8F3-8240-95EB-DE1F6F81C349}" type="presParOf" srcId="{1D3F560C-301B-434B-A1FD-2D4533B00084}" destId="{CD750812-B108-564F-992D-C437D68E95A1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{1CDB415D-1AC5-7D49-AF5E-A7142C8DE691}" type="presParOf" srcId="{CD750812-B108-564F-992D-C437D68E95A1}" destId="{085C6D68-61FF-5147-81E0-9AEF37B2ECCB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{E666623E-8EC2-2847-A6EC-C338EAB7DE0C}" type="presParOf" srcId="{1D3F560C-301B-434B-A1FD-2D4533B00084}" destId="{AE3ABCE3-88A7-4D40-8B8A-323DD095ABDD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{C7C5E201-29A7-444B-9114-B0A008955617}" type="presParOf" srcId="{AE3ABCE3-88A7-4D40-8B8A-323DD095ABDD}" destId="{69AC3AD2-ED21-5344-AD1D-FDFEEE7C4C5B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{51D0CE02-451B-DD41-9E60-2CD40DABFE87}" type="presParOf" srcId="{AE3ABCE3-88A7-4D40-8B8A-323DD095ABDD}" destId="{4213F435-3482-8244-A9A1-055C2931906F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{FB5B88A8-F3FD-FE4F-BA55-6B5117C30772}" type="presParOf" srcId="{DEA98603-1475-6643-B90D-B4C5B3BB2727}" destId="{11AB213E-7F90-F141-9549-20DEA56EEBBD}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{883E5E9E-CBE2-A347-9E03-E1640974CED6}" type="presParOf" srcId="{11AB213E-7F90-F141-9549-20DEA56EEBBD}" destId="{C89AF06C-5711-7D48-A237-493096B9D115}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{C420410E-F767-9641-A0E9-C7415D0FB809}" type="presParOf" srcId="{DEA98603-1475-6643-B90D-B4C5B3BB2727}" destId="{EDD11DE7-1B17-6D40-912C-B73F3838AC65}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{C59DCAAE-A4FD-A943-AC98-38E03569DB2F}" type="presParOf" srcId="{EDD11DE7-1B17-6D40-912C-B73F3838AC65}" destId="{080C10A4-0453-4948-B1F3-2DFE4B8C8CE4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{97F2577E-4674-0747-AB72-1AC1E7ED21EC}" type="presParOf" srcId="{EDD11DE7-1B17-6D40-912C-B73F3838AC65}" destId="{F045EA84-A9CB-8941-BD1C-77E82ACA70BC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{BFB3D4F1-B3BA-6C4C-A490-0D0FD66FC246}" type="presParOf" srcId="{DEA98603-1475-6643-B90D-B4C5B3BB2727}" destId="{E4A90812-59D6-D34C-91E1-E3C466D41D1B}" srcOrd="6" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{93024D41-19E0-7E40-875A-6685672443C2}" type="presParOf" srcId="{E4A90812-59D6-D34C-91E1-E3C466D41D1B}" destId="{6B763081-220F-944D-96A7-37B055955D48}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{551460DB-4038-1042-8594-04AB5F6383A7}" type="presParOf" srcId="{DEA98603-1475-6643-B90D-B4C5B3BB2727}" destId="{8ED44C45-8E58-4B40-B6C1-F9FAD4C31112}" srcOrd="7" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{21963943-0C90-474A-961E-9190F4D80A3B}" type="presParOf" srcId="{8ED44C45-8E58-4B40-B6C1-F9FAD4C31112}" destId="{BBEAC981-0AA3-BE43-933A-96CDBD00C9A2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{F6F15902-FE15-BC41-A44D-CE1E010BC449}" type="presParOf" srcId="{8ED44C45-8E58-4B40-B6C1-F9FAD4C31112}" destId="{4F1BB898-E113-A845-BCED-21337085BC33}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{5E008749-8578-3940-9A9C-9DD60C881FCD}" type="presParOf" srcId="{DEA98603-1475-6643-B90D-B4C5B3BB2727}" destId="{FE83888B-4547-9642-A036-470E88BA049D}" srcOrd="8" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{420792F1-B0A1-D047-83F0-0B615B1A7651}" type="presParOf" srcId="{FE83888B-4547-9642-A036-470E88BA049D}" destId="{A77D1BEF-37F9-7242-91A8-9D907E7CC0B4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{EF2AD85D-D99E-2E42-8628-C6886A00CEF1}" type="presParOf" srcId="{DEA98603-1475-6643-B90D-B4C5B3BB2727}" destId="{DC1F6217-0341-D948-9642-F637E5F7E362}" srcOrd="9" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{DF02848E-5147-9D43-A94B-4CD63FD744FD}" type="presParOf" srcId="{DC1F6217-0341-D948-9642-F637E5F7E362}" destId="{567E4FBD-1A65-6B48-8A6D-F72A7955CE15}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{D01358B0-E225-5341-BECD-A06C4236B816}" type="presParOf" srcId="{DC1F6217-0341-D948-9642-F637E5F7E362}" destId="{4064B30A-9269-F742-B21A-E7536FBB9B43}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{678B791F-859B-454D-A0ED-B7ECDA9E57E9}" type="presParOf" srcId="{598F85C8-C84D-C143-8558-EE261698AAD1}" destId="{199187A2-043D-8540-A3D5-F92622E95501}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{518D0565-2299-284F-AA82-FF534E3C296D}" type="presParOf" srcId="{199187A2-043D-8540-A3D5-F92622E95501}" destId="{968DCEBD-CF0C-D74A-A666-31158F65E182}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{C2F29CDA-428E-7149-A3E7-07DF46EAE0A1}" type="presParOf" srcId="{598F85C8-C84D-C143-8558-EE261698AAD1}" destId="{6C1E8FD9-477E-684D-B4BA-F9AD3239AD3B}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
@@ -2767,29 +3195,24 @@
     <dgm:cxn modelId="{5771D5EE-AA4B-DD4B-820A-F9197B50B776}" type="presParOf" srcId="{6F7BF31D-8E73-9A4D-8E76-ECB3E38C37A1}" destId="{120D2242-86A1-A442-A1C7-C33EE729768D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{B3C48AA0-02D6-CC44-B385-DF2F9D896A19}" type="presParOf" srcId="{120D2242-86A1-A442-A1C7-C33EE729768D}" destId="{9F55E6EF-25E4-B542-8DEE-25656226127F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{0C44FCCD-0CE9-F64C-8DBB-2ADAB8527C5A}" type="presParOf" srcId="{120D2242-86A1-A442-A1C7-C33EE729768D}" destId="{645BCC2E-DF41-B64E-8B89-6603B642452E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{0BA518FC-6B57-9748-8EC1-94628AFF3492}" type="presParOf" srcId="{598F85C8-C84D-C143-8558-EE261698AAD1}" destId="{A608BD11-03C6-9149-9A0C-9460A3FE91FB}" srcOrd="6" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{DEC875E8-46B4-114D-ACF6-BA5AE03474FD}" type="presParOf" srcId="{A608BD11-03C6-9149-9A0C-9460A3FE91FB}" destId="{D5068B54-DECB-5C40-8C43-3E238EA1A151}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{ED73FD3D-E233-1949-B151-16AC88F81B52}" type="presParOf" srcId="{598F85C8-C84D-C143-8558-EE261698AAD1}" destId="{85DB200A-1A2A-4E49-BB42-9798DD0F7491}" srcOrd="7" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{7C47A739-5F3D-7840-BD05-9C1E20CD99CC}" type="presParOf" srcId="{85DB200A-1A2A-4E49-BB42-9798DD0F7491}" destId="{D90297FE-FAC7-9042-A8CC-4C7D825B33BF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{195C7E12-E001-2943-A75B-3581C1976759}" type="presParOf" srcId="{85DB200A-1A2A-4E49-BB42-9798DD0F7491}" destId="{43967FCB-616D-F84C-8966-503D83458021}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{BD68A33B-159A-B448-9159-EEFD64BA5750}" type="presParOf" srcId="{43967FCB-616D-F84C-8966-503D83458021}" destId="{96B1CDE0-C35A-CB43-9A64-AE7BDFB44B3E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{5A771299-151D-1E4A-A905-D1F2ED9D691A}" type="presParOf" srcId="{96B1CDE0-C35A-CB43-9A64-AE7BDFB44B3E}" destId="{769BF5E9-2773-7642-A2AF-516B0418FC0F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{C62D083F-92A6-D74E-BD42-D3AB6AF98A0C}" type="presParOf" srcId="{43967FCB-616D-F84C-8966-503D83458021}" destId="{BA13AD0C-76AA-5843-A605-E16AAE70ED9A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{92E5F7BF-28EF-F344-9BBF-3B1CEC51160E}" type="presParOf" srcId="{BA13AD0C-76AA-5843-A605-E16AAE70ED9A}" destId="{9FDC99B0-D551-004A-864C-6DCAFEB88B76}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{3E32EC9F-F3F7-D94A-A178-DDC520DEF94F}" type="presParOf" srcId="{BA13AD0C-76AA-5843-A605-E16AAE70ED9A}" destId="{F767CC2E-1D10-8745-9E1F-96823794A4C7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{A59C04C2-1F9D-1247-B06E-5CCAC11366DC}" type="presParOf" srcId="{598F85C8-C84D-C143-8558-EE261698AAD1}" destId="{49C1BB80-7116-0243-8559-F49FE35EAC8C}" srcOrd="8" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{B7A53937-DA31-1246-A81F-77B8C5309BFA}" type="presParOf" srcId="{49C1BB80-7116-0243-8559-F49FE35EAC8C}" destId="{7DED3A20-7857-564A-9D1E-9551D5E2DF6D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{71C7002A-3C57-FB42-B3F4-24D8A35313D4}" type="presParOf" srcId="{598F85C8-C84D-C143-8558-EE261698AAD1}" destId="{9289C2FC-A477-3647-940B-134169176A90}" srcOrd="9" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{3E90FB9F-A524-C044-A125-7C4BE3A20515}" type="presParOf" srcId="{9289C2FC-A477-3647-940B-134169176A90}" destId="{96296898-BE98-0247-83BE-61F5D3D682F5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{058B1A44-6814-714B-BAA5-8491BC02C3CF}" type="presParOf" srcId="{9289C2FC-A477-3647-940B-134169176A90}" destId="{845FD99B-46AA-D04B-996F-EFB1B6DC0135}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{7B58A84F-7F49-5A4E-A640-30EA4DA7E7C9}" type="presParOf" srcId="{845FD99B-46AA-D04B-996F-EFB1B6DC0135}" destId="{04C15EBF-48BF-2D4C-BF9B-0823F14313EF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{18B83132-77CE-9B45-8BF1-3E687A970297}" type="presParOf" srcId="{04C15EBF-48BF-2D4C-BF9B-0823F14313EF}" destId="{C08397E8-4357-1040-B413-6547DDCD0CDD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{8F75A1B9-7B12-B348-92A8-2088AA219BC5}" type="presParOf" srcId="{845FD99B-46AA-D04B-996F-EFB1B6DC0135}" destId="{1DED0AA9-3924-334A-8D8D-33478E7657B0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{190B93DC-BFBC-364E-8256-F1D333FF9B95}" type="presParOf" srcId="{1DED0AA9-3924-334A-8D8D-33478E7657B0}" destId="{98E56F84-7B9F-E448-A77F-BECF084C032C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{811DBF6F-55B5-994F-BAB2-1755061A0E07}" type="presParOf" srcId="{1DED0AA9-3924-334A-8D8D-33478E7657B0}" destId="{4F99EDBC-C258-2349-A0FD-89D18599CDD0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{E81D27EC-A850-B344-8876-89526B00B9BB}" type="presParOf" srcId="{B1B8291F-AF33-5D48-99F4-EFCEA4F477B2}" destId="{F2B8E9EC-9E8D-EF4F-8069-8CF8FD8833B2}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{4F350975-3C9B-E243-AD3E-7CCB195F2259}" type="presParOf" srcId="{B1B8291F-AF33-5D48-99F4-EFCEA4F477B2}" destId="{622176D4-0F63-4441-9655-4E39F2D4E064}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{5415E7FE-B8AF-134D-8B05-30F1C27B95F2}" type="presParOf" srcId="{622176D4-0F63-4441-9655-4E39F2D4E064}" destId="{9CBE3C3D-6969-BA40-9AFD-12D8A930CA33}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{75DD7551-E57A-9748-B944-23A6F499939B}" type="presParOf" srcId="{B1B8291F-AF33-5D48-99F4-EFCEA4F477B2}" destId="{4F9608FB-4CF1-644A-A181-4483BAED8A3B}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{931A4295-4F05-E645-A06F-98C4D7A69A14}" type="presParOf" srcId="{4F9608FB-4CF1-644A-A181-4483BAED8A3B}" destId="{F9CE8C8D-1F59-A546-857D-5DCA77549F01}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{B1218134-69D8-7D46-A216-7E0F7BAA8134}" type="presParOf" srcId="{4F9608FB-4CF1-644A-A181-4483BAED8A3B}" destId="{EB59BBE9-3A43-2145-809F-98F8ECA7D98F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{795FE339-6EAC-D944-8374-B3472E817990}" type="presParOf" srcId="{EB59BBE9-3A43-2145-809F-98F8ECA7D98F}" destId="{EC671750-0F9F-144E-B9B1-0F71732606F0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{856E7D9E-BD3B-AD4D-89CC-0C04A1C1773D}" type="presParOf" srcId="{EC671750-0F9F-144E-B9B1-0F71732606F0}" destId="{56D4E8B8-277E-6C4C-B5C0-2B77C4634751}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{AA402E8C-B423-6745-9896-D9FE7E06933F}" type="presParOf" srcId="{EB59BBE9-3A43-2145-809F-98F8ECA7D98F}" destId="{568918D7-6938-E249-9E2B-254463D3E59B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{AB8298B6-14EC-1149-B73B-05629C3AD1EA}" type="presParOf" srcId="{568918D7-6938-E249-9E2B-254463D3E59B}" destId="{DFF22F0D-7EB3-DB46-B99E-239BB764C2DC}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{580529CD-6F99-1D47-863B-3CC50E608D68}" type="presParOf" srcId="{568918D7-6938-E249-9E2B-254463D3E59B}" destId="{F519F3D3-72EC-D546-97C3-75849C2CA254}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{EAA64E1A-8D95-8F48-9DE5-BF4C38F9FB6A}" type="presParOf" srcId="{EB59BBE9-3A43-2145-809F-98F8ECA7D98F}" destId="{9FA40A36-B6C2-5140-97C1-947018A2B70F}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{8C211F93-FA35-414F-A100-5A75AFECA4C9}" type="presParOf" srcId="{9FA40A36-B6C2-5140-97C1-947018A2B70F}" destId="{5E4F97FA-974D-8845-A8FE-60389B8C4834}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{3C49D9C9-1DF5-384D-9765-AFB2D2A3D767}" type="presParOf" srcId="{EB59BBE9-3A43-2145-809F-98F8ECA7D98F}" destId="{C0072E1F-3A0C-0940-A1CD-530FB2B10CD1}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{088ED4C8-52C1-1244-ACDD-1E68931A9176}" type="presParOf" srcId="{C0072E1F-3A0C-0940-A1CD-530FB2B10CD1}" destId="{0963A656-C5DC-AB41-8DEE-D65A14EA566F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{768361AF-9EFA-DB4A-AE48-2E986CCE0501}" type="presParOf" srcId="{C0072E1F-3A0C-0940-A1CD-530FB2B10CD1}" destId="{63BE4F91-CBE1-B542-8CD4-1BA6649119A2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{E81D27EC-A850-B344-8876-89526B00B9BB}" type="presParOf" srcId="{B1B8291F-AF33-5D48-99F4-EFCEA4F477B2}" destId="{F2B8E9EC-9E8D-EF4F-8069-8CF8FD8833B2}" srcOrd="6" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{3748A6D0-F0F2-3E48-9419-1915A45B5327}" type="presParOf" srcId="{F2B8E9EC-9E8D-EF4F-8069-8CF8FD8833B2}" destId="{1A86F6FD-7823-CA48-AB5A-F31345841067}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
-    <dgm:cxn modelId="{76F1D2E0-5CED-8B4A-AE1B-00682E9F13EC}" type="presParOf" srcId="{B1B8291F-AF33-5D48-99F4-EFCEA4F477B2}" destId="{D5E11BF9-817C-CD42-900E-A9BC452624B0}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
+    <dgm:cxn modelId="{76F1D2E0-5CED-8B4A-AE1B-00682E9F13EC}" type="presParOf" srcId="{B1B8291F-AF33-5D48-99F4-EFCEA4F477B2}" destId="{D5E11BF9-817C-CD42-900E-A9BC452624B0}" srcOrd="7" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{2333F10C-C2A4-C345-AFAF-6FD59C028DDB}" type="presParOf" srcId="{D5E11BF9-817C-CD42-900E-A9BC452624B0}" destId="{53EE5430-A405-0C45-8C3D-56B9B7B4C5EE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{628EDEAF-16A2-584E-89B2-E16DDE07C101}" type="presParOf" srcId="{D5E11BF9-817C-CD42-900E-A9BC452624B0}" destId="{0B0444E0-1C9D-7944-896B-7915BA26BAB2}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
     <dgm:cxn modelId="{89AEA3C5-9298-364E-9FCA-2BFEBB5C7869}" type="presParOf" srcId="{0B0444E0-1C9D-7944-896B-7915BA26BAB2}" destId="{CF5C0BC9-1C55-6D44-9740-9A1957FD4485}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy2"/>
@@ -2838,8 +3261,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="1342256" y="3752876"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="1315591" y="3690056"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -2899,12 +3322,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2916,14 +3339,14 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" kern="1200"/>
+            <a:rPr lang="fr-FR" sz="700" kern="1200"/>
             <a:t>Projet HELP</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="1359625" y="3770245"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="1329497" y="3703962"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{1AEC4C7F-8B5D-9C4A-A0BA-DF9BE251EB21}">
@@ -2932,9 +3355,9 @@
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm rot="16791948">
-          <a:off x="1381084" y="2678247"/>
-          <a:ext cx="2768829" cy="14392"/>
+        <a:xfrm rot="16613897">
+          <a:off x="873862" y="2352028"/>
+          <a:ext cx="3162470" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2945,10 +3368,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="2768829" y="7196"/>
+                <a:pt x="3162470" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2986,7 +3409,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="355600">
+          <a:pPr lvl="0" algn="ctr" defTabSz="266700">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2997,12 +3420,12 @@
               <a:spcPct val="35000"/>
             </a:spcAft>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR" sz="800" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2696278" y="2616223"/>
-        <a:ext cx="138441" cy="138441"/>
+        <a:off x="2376035" y="2278603"/>
+        <a:ext cx="158123" cy="158123"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{02E0FECA-2589-C94E-8421-1373276E6CD0}">
@@ -3012,8 +3435,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3002706" y="1024993"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="2645015" y="550479"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3073,12 +3496,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3090,15 +3513,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>FP1 : Enregistrer les données nécessaire à la détection de l'individu</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP1 : Enregistrer les données nécessaire à la détection du mouvement de l'oeil</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3020075" y="1042362"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="2658921" y="564385"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{97838F66-388F-334E-8C48-6883CD119D60}">
@@ -3107,9 +3530,9 @@
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm rot="17692822">
-          <a:off x="3862144" y="802828"/>
-          <a:ext cx="1127611" cy="14392"/>
+        <a:xfrm rot="18289469">
+          <a:off x="3451953" y="509233"/>
+          <a:ext cx="665135" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3120,10 +3543,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1127611" y="7196"/>
+                <a:pt x="665135" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3176,8 +3599,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4397759" y="781833"/>
-        <a:ext cx="56380" cy="56380"/>
+        <a:off x="3767893" y="498241"/>
+        <a:ext cx="33256" cy="33256"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E51D9155-7752-9D41-957A-949CC75EB761}">
@@ -3187,8 +3610,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4663157" y="2037"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="3974439" y="4465"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3248,12 +3671,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3265,15 +3688,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
             <a:t>FP11 : Enregistrer l'individu</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4680526" y="19406"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="3988345" y="18371"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{9F3C9693-87FA-7F45-B58A-F884460F249C}">
@@ -3283,8 +3706,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5849193" y="291350"/>
-          <a:ext cx="474414" cy="14392"/>
+          <a:off x="4924027" y="236226"/>
+          <a:ext cx="379835" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3295,10 +3718,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="474414" y="7196"/>
+                <a:pt x="379835" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3351,8 +3774,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6074540" y="286685"/>
-        <a:ext cx="23720" cy="23720"/>
+        <a:off x="5104449" y="232366"/>
+        <a:ext cx="18991" cy="18991"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{09A02069-0039-4049-80CB-8B6C97B26549}">
@@ -3362,8 +3785,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6323607" y="2037"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="5303863" y="4465"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3423,12 +3846,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3440,15 +3863,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
             <a:t>Caméra vers l'individu</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6340976" y="19406"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="5317769" y="18371"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{6880828A-3410-E644-A3C4-2294177CC41C}">
@@ -3457,9 +3880,9 @@
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm rot="19457599">
-          <a:off x="4133828" y="1143813"/>
-          <a:ext cx="584243" cy="14392"/>
+        <a:xfrm>
+          <a:off x="3594603" y="782240"/>
+          <a:ext cx="379835" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3470,10 +3893,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="584243" y="7196"/>
+                <a:pt x="379835" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3526,8 +3949,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4411343" y="1136403"/>
-        <a:ext cx="29212" cy="29212"/>
+        <a:off x="3775025" y="778380"/>
+        <a:ext cx="18991" cy="18991"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{22159CD9-4EC1-E544-98E6-9AD9F99F03AF}">
@@ -3537,8 +3960,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4663157" y="684007"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="3974439" y="550479"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3598,12 +4021,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3615,15 +4038,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
             <a:t>FP12 : Enregistrer les données nécessaires au calcul de la distance de l'individu à l'interface</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4680526" y="701376"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="3988345" y="564385"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{CB5AFF4C-0CEC-F643-96B6-DAC4ED874BEC}">
@@ -3633,8 +4056,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5849193" y="973320"/>
-          <a:ext cx="474414" cy="14392"/>
+          <a:off x="4924027" y="782240"/>
+          <a:ext cx="379835" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3645,10 +4068,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="474414" y="7196"/>
+                <a:pt x="379835" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3701,8 +4124,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6074540" y="968656"/>
-        <a:ext cx="23720" cy="23720"/>
+        <a:off x="5104449" y="778380"/>
+        <a:ext cx="18991" cy="18991"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{5A6C940B-8E0D-2541-B4EE-37D9893DC81C}">
@@ -3712,8 +4135,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6323607" y="684007"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="5303863" y="550479"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3773,12 +4196,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3790,15 +4213,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
             <a:t>Caméras tournées vers l'écran</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6340976" y="701376"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="5317769" y="564385"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E51D49A7-6AFC-F04F-9B53-612EDC5C173D}">
@@ -3807,9 +4230,9 @@
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm rot="2142401">
-          <a:off x="4133828" y="1484798"/>
-          <a:ext cx="584243" cy="14392"/>
+        <a:xfrm rot="3310531">
+          <a:off x="3451953" y="1055246"/>
+          <a:ext cx="665135" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3820,10 +4243,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="584243" y="7196"/>
+                <a:pt x="665135" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3876,8 +4299,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4411343" y="1477388"/>
-        <a:ext cx="29212" cy="29212"/>
+        <a:off x="3767893" y="1044254"/>
+        <a:ext cx="33256" cy="33256"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{ED82EB34-8097-994C-90F2-D4621919418A}">
@@ -3887,8 +4310,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4663157" y="1365978"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="3974439" y="1096492"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -3948,12 +4371,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3965,15 +4388,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
             <a:t>FP13 : Relayer les données à la carte de traitement</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4680526" y="1383347"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="3988345" y="1110398"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{7FC46335-8ED1-2E49-A7BE-E54D41297FCD}">
@@ -3983,8 +4406,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5849193" y="1655291"/>
-          <a:ext cx="474414" cy="14392"/>
+          <a:off x="4924027" y="1328253"/>
+          <a:ext cx="379835" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3995,10 +4418,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="474414" y="7196"/>
+                <a:pt x="379835" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4051,8 +4474,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6074540" y="1650627"/>
-        <a:ext cx="23720" cy="23720"/>
+        <a:off x="5104449" y="1324393"/>
+        <a:ext cx="18991" cy="18991"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{743C9E64-CA35-3346-BD28-35C33D90F652}">
@@ -4062,8 +4485,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6323607" y="1365978"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="5303863" y="1096492"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4123,12 +4546,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4140,26 +4563,26 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
             <a:t>Système sans fil / cable</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6340976" y="1383347"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="5317769" y="1110398"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{EAE6DA3D-6DCE-8B43-86D6-453237F6F64F}">
+    <dsp:sp modelId="{9214EDCC-7637-FA4F-A663-9416C90A1781}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm rot="3907178">
-          <a:off x="3862144" y="1825784"/>
-          <a:ext cx="1127611" cy="14392"/>
+        <a:xfrm rot="18770822">
+          <a:off x="2175824" y="3717062"/>
+          <a:ext cx="558545" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4170,10 +4593,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1127611" y="7196"/>
+                <a:pt x="558545" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4182,7 +4605,7 @@
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
+              <a:shade val="60000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -4226,19 +4649,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4397759" y="1804790"/>
-        <a:ext cx="56380" cy="56380"/>
+        <a:off x="2441133" y="3708734"/>
+        <a:ext cx="27927" cy="27927"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{AFB00BA5-37D3-4D49-ABEF-E265A327F349}">
+    <dsp:sp modelId="{B895C344-133F-4340-80A0-685E27E999D6}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4663157" y="2047949"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="2645015" y="3280546"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4298,12 +4721,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4315,26 +4738,26 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>FP14 : Compresser les données</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP2 : Transférer et traiter les données enregistrées</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4680526" y="2065318"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="2658921" y="3294452"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{DA2BBBC5-96AE-D245-B903-7F481B166D03}">
+    <dsp:sp modelId="{F07A7E6F-36EA-9743-8C2B-402848A63CFF}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5849193" y="2337262"/>
-          <a:ext cx="474414" cy="14392"/>
+        <a:xfrm rot="16983315">
+          <a:off x="2943770" y="2693287"/>
+          <a:ext cx="1681502" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4345,10 +4768,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="474414" y="7196"/>
+                <a:pt x="1681502" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4386,7 +4809,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="266700">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4397,23 +4820,23 @@
               <a:spcPct val="35000"/>
             </a:spcAft>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6074540" y="2332598"/>
-        <a:ext cx="23720" cy="23720"/>
+        <a:off x="3742483" y="2656885"/>
+        <a:ext cx="84075" cy="84075"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{64CE6CC6-6955-1F47-A64D-5C4536E66E8E}">
+    <dsp:sp modelId="{D0686948-65B5-CE4B-99C1-9EB45F62AC5F}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6323607" y="2047949"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="3974439" y="1642505"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4473,12 +4896,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4490,26 +4913,26 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>Carte de traitement</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP21 : Transmettre le signal compressé</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6340976" y="2065318"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="3988345" y="1656411"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{9214EDCC-7637-FA4F-A663-9416C90A1781}">
+    <dsp:sp modelId="{0458EB9C-8D95-A54A-BBFE-4EB0E4F471AD}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm rot="2142401">
-          <a:off x="2473377" y="4212682"/>
-          <a:ext cx="584243" cy="14392"/>
+        <a:xfrm>
+          <a:off x="4924027" y="1874267"/>
+          <a:ext cx="379835" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4520,10 +4943,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="584243" y="7196"/>
+                <a:pt x="379835" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4532,7 +4955,7 @@
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -4576,19 +4999,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2750893" y="4205272"/>
-        <a:ext cx="29212" cy="29212"/>
+        <a:off x="5104449" y="1870407"/>
+        <a:ext cx="18991" cy="18991"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{B895C344-133F-4340-80A0-685E27E999D6}">
+    <dsp:sp modelId="{3E1A4BA4-A92F-724C-AE87-430A70601B53}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3002706" y="4093861"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="5303863" y="1642505"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4648,12 +5071,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4665,26 +5088,26 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>FP2 : Transférer et traiter les données enregistrées</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>Système sans fil</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3020075" y="4111230"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="5317769" y="1656411"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{F07A7E6F-36EA-9743-8C2B-402848A63CFF}">
+    <dsp:sp modelId="{36D788C9-8DB5-D74D-BDE6-649BA5A5D5B8}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm rot="17350740">
-          <a:off x="3703903" y="3701203"/>
-          <a:ext cx="1444093" cy="14392"/>
+        <a:xfrm>
+          <a:off x="3594603" y="3512307"/>
+          <a:ext cx="379835" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4695,10 +5118,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1444093" y="7196"/>
+                <a:pt x="379835" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4751,19 +5174,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4389847" y="3672297"/>
-        <a:ext cx="72204" cy="72204"/>
+        <a:off x="3775025" y="3508447"/>
+        <a:ext cx="18991" cy="18991"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{D0686948-65B5-CE4B-99C1-9EB45F62AC5F}">
+    <dsp:sp modelId="{C6AA8951-971D-8D46-A6B7-A3287247CC64}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4663157" y="2729920"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="3974439" y="3280546"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4823,12 +5246,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4840,26 +5263,25 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>FP21 : Transmettre le signal compressé</a:t>
+            <a:rPr lang="fr-FR" sz="700" kern="1200"/>
+            <a:t>FP22 : Détecter l'individu et ses mouvements</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4680526" y="2747289"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="3988345" y="3294452"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{0458EB9C-8D95-A54A-BBFE-4EB0E4F471AD}">
+    <dsp:sp modelId="{5DFE3D87-3E56-EE42-9E29-FC62E4F1FBAE}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5849193" y="3019233"/>
-          <a:ext cx="474414" cy="14392"/>
+        <a:xfrm rot="17350740">
+          <a:off x="4535845" y="2966293"/>
+          <a:ext cx="1156199" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4870,10 +5292,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="474414" y="7196"/>
+                <a:pt x="1156199" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -4926,19 +5348,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6074540" y="3014568"/>
-        <a:ext cx="23720" cy="23720"/>
+        <a:off x="5085040" y="2943024"/>
+        <a:ext cx="57809" cy="57809"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{3E1A4BA4-A92F-724C-AE87-430A70601B53}">
+    <dsp:sp modelId="{8A60DE61-E72C-854C-836C-D906D1A70AB7}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6323607" y="2729920"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="5303863" y="2188519"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -4998,12 +5420,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5015,15 +5437,14 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>Système sans fil</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP221 : Détecter l'individu</a:t>
           </a:r>
-          <a:endParaRPr lang="fr-FR" sz="900" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6340976" y="2747289"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="5317769" y="2202425"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{25F721B1-6D69-F140-A42C-4801B2DBF60A}">
@@ -5033,8 +5454,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="18289469">
-          <a:off x="4010572" y="4042189"/>
-          <a:ext cx="830754" cy="14392"/>
+          <a:off x="4781377" y="3239300"/>
+          <a:ext cx="665135" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5045,10 +5466,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="830754" y="7196"/>
+                <a:pt x="665135" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5101,8 +5522,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4405181" y="4028616"/>
-        <a:ext cx="41537" cy="41537"/>
+        <a:off x="5097317" y="3228308"/>
+        <a:ext cx="33256" cy="33256"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{84D18324-7849-AF4F-A07E-80E004C8B650}">
@@ -5112,8 +5533,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4663157" y="3411890"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="5303863" y="2734532"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5173,12 +5594,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5190,14 +5611,14 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>FP22 : Détecter l'oeil</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP222 : Détecter l'oeil</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4680526" y="3429259"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="5317769" y="2748438"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{CD750812-B108-564F-992D-C437D68E95A1}">
@@ -5207,8 +5628,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5849193" y="3701203"/>
-          <a:ext cx="474414" cy="14392"/>
+          <a:off x="6253451" y="2966293"/>
+          <a:ext cx="379835" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5219,10 +5640,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="474414" y="7196"/>
+                <a:pt x="379835" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5275,8 +5696,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6074540" y="3696539"/>
-        <a:ext cx="23720" cy="23720"/>
+        <a:off x="6433873" y="2962433"/>
+        <a:ext cx="18991" cy="18991"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{69AC3AD2-ED21-5344-AD1D-FDFEEE7C4C5B}">
@@ -5286,8 +5707,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6323607" y="3411890"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="6633287" y="2734532"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5347,12 +5768,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5364,25 +5785,25 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
             <a:t>Logiciel d'algorithmique</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6340976" y="3429259"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="6647193" y="2748438"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{199187A2-043D-8540-A3D5-F92622E95501}">
+    <dsp:sp modelId="{11AB213E-7F90-F141-9549-20DEA56EEBBD}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4188742" y="4383174"/>
-          <a:ext cx="474414" cy="14392"/>
+          <a:off x="4924027" y="3512307"/>
+          <a:ext cx="379835" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5393,10 +5814,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="474414" y="7196"/>
+                <a:pt x="379835" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5449,19 +5870,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4414089" y="4378510"/>
-        <a:ext cx="23720" cy="23720"/>
+        <a:off x="5104449" y="3508447"/>
+        <a:ext cx="18991" cy="18991"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{2A221514-4A03-4B45-B5AF-749FB8232375}">
+    <dsp:sp modelId="{080C10A4-0453-4948-B1F3-2DFE4B8C8CE4}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4663157" y="4093861"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="5303863" y="3280546"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5521,12 +5942,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5538,25 +5959,25 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>FP23 : Calculer la distance entre l'individu et l'interface</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP223 : Détecter la pupille</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4680526" y="4111230"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="5317769" y="3294452"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{5DA24466-CB9E-0F43-B8A3-FA63AE383C78}">
+    <dsp:sp modelId="{E4A90812-59D6-D34C-91E1-E3C466D41D1B}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5849193" y="4383174"/>
-          <a:ext cx="474414" cy="14392"/>
+        <a:xfrm rot="3310531">
+          <a:off x="4781377" y="3785314"/>
+          <a:ext cx="665135" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5567,10 +5988,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="474414" y="7196"/>
+                <a:pt x="665135" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5623,19 +6044,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6074540" y="4378510"/>
-        <a:ext cx="23720" cy="23720"/>
+        <a:off x="5097317" y="3774321"/>
+        <a:ext cx="33256" cy="33256"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{9F55E6EF-25E4-B542-8DEE-25656226127F}">
+    <dsp:sp modelId="{BBEAC981-0AA3-BE43-933A-96CDBD00C9A2}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6323607" y="4093861"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="5303863" y="3826559"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5695,12 +6116,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5712,25 +6133,25 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>Logiciel d'algorithmique</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP224 : Détecter le mouvement de la pupille</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6340976" y="4111230"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="5317769" y="3840465"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{A608BD11-03C6-9149-9A0C-9460A3FE91FB}">
+    <dsp:sp modelId="{FE83888B-4547-9642-A036-470E88BA049D}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm rot="3310531">
-          <a:off x="4010572" y="4724160"/>
-          <a:ext cx="830754" cy="14392"/>
+        <a:xfrm rot="4249260">
+          <a:off x="4535845" y="4058320"/>
+          <a:ext cx="1156199" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5741,10 +6162,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="830754" y="7196"/>
+                <a:pt x="1156199" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5797,19 +6218,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4405181" y="4710587"/>
-        <a:ext cx="41537" cy="41537"/>
+        <a:off x="5085040" y="4035051"/>
+        <a:ext cx="57809" cy="57809"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{D90297FE-FAC7-9042-A8CC-4C7D825B33BF}">
+    <dsp:sp modelId="{567E4FBD-1A65-6B48-8A6D-F72A7955CE15}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4663157" y="4775832"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="5303863" y="4372572"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -5869,12 +6290,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5886,25 +6307,25 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>FP24 : Analyser le mouvement de la pupille</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP225 : Détecter le clignement de l'oeil</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4680526" y="4793201"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="5317769" y="4386478"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{96B1CDE0-C35A-CB43-9A64-AE7BDFB44B3E}">
+    <dsp:sp modelId="{199187A2-043D-8540-A3D5-F92622E95501}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5849193" y="5065145"/>
-          <a:ext cx="474414" cy="14392"/>
+        <a:xfrm rot="4616685">
+          <a:off x="2943770" y="4331327"/>
+          <a:ext cx="1681502" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5915,10 +6336,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="474414" y="7196"/>
+                <a:pt x="1681502" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -5956,7 +6377,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="266700">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5967,23 +6388,23 @@
               <a:spcPct val="35000"/>
             </a:spcAft>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6074540" y="5060481"/>
-        <a:ext cx="23720" cy="23720"/>
+        <a:off x="3742483" y="4294925"/>
+        <a:ext cx="84075" cy="84075"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{9FDC99B0-D551-004A-864C-6DCAFEB88B76}">
+    <dsp:sp modelId="{2A221514-4A03-4B45-B5AF-749FB8232375}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6323607" y="4775832"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="3974439" y="4918586"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6043,12 +6464,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6060,25 +6481,25 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>Logiciel d'algorithmique</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP23 : Calculer la distance entre l'individu et l'interface</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6340976" y="4793201"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="3988345" y="4932492"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{49C1BB80-7116-0243-8559-F49FE35EAC8C}">
+    <dsp:sp modelId="{5DA24466-CB9E-0F43-B8A3-FA63AE383C78}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm rot="4249260">
-          <a:off x="3703903" y="5065145"/>
-          <a:ext cx="1444093" cy="14392"/>
+        <a:xfrm>
+          <a:off x="4924027" y="5150347"/>
+          <a:ext cx="379835" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6089,10 +6510,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="1444093" y="7196"/>
+                <a:pt x="379835" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6145,19 +6566,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4389847" y="5036239"/>
-        <a:ext cx="72204" cy="72204"/>
+        <a:off x="5104449" y="5146487"/>
+        <a:ext cx="18991" cy="18991"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{96296898-BE98-0247-83BE-61F5D3D682F5}">
+    <dsp:sp modelId="{9F55E6EF-25E4-B542-8DEE-25656226127F}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4663157" y="5457803"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="5303863" y="4918586"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6217,12 +6638,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6234,25 +6655,25 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>FP25 : Déduire l'action à exécuter</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>Logiciel d'algorithmique</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4680526" y="5475172"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="5317769" y="4932492"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{04C15EBF-48BF-2D4C-BF9B-0823F14313EF}">
+    <dsp:sp modelId="{622176D4-0F63-4441-9655-4E39F2D4E064}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5849193" y="5747116"/>
-          <a:ext cx="474414" cy="14392"/>
+        <a:xfrm rot="4769441">
+          <a:off x="1413855" y="4945592"/>
+          <a:ext cx="2082483" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6263,10 +6684,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="474414" y="7196"/>
+                <a:pt x="2082483" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6275,7 +6696,7 @@
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
+              <a:shade val="60000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -6304,7 +6725,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="266700">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6315,23 +6736,23 @@
               <a:spcPct val="35000"/>
             </a:spcAft>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6074540" y="5742451"/>
-        <a:ext cx="23720" cy="23720"/>
+        <a:off x="2403035" y="4899166"/>
+        <a:ext cx="104124" cy="104124"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{98E56F84-7B9F-E448-A77F-BECF084C032C}">
+    <dsp:sp modelId="{F9CE8C8D-1F59-A546-857D-5DCA77549F01}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6323607" y="5457803"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="2645015" y="5737606"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6391,12 +6812,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6408,25 +6829,25 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>Logiciel d'algorithmique</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP3 : Interpréter les données pour déduire l'action à exécuter</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6340976" y="5475172"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="2658921" y="5751512"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{F2B8E9EC-9E8D-EF4F-8069-8CF8FD8833B2}">
+    <dsp:sp modelId="{EC671750-0F9F-144E-B9B1-0F71732606F0}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm rot="4808052">
-          <a:off x="1381084" y="5406130"/>
-          <a:ext cx="2768829" cy="14392"/>
+        <a:xfrm rot="19457599">
+          <a:off x="3550637" y="5832864"/>
+          <a:ext cx="467768" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6437,10 +6858,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="2768829" y="7196"/>
+                <a:pt x="467768" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6449,7 +6870,7 @@
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
+              <a:shade val="80000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -6478,7 +6899,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="355600">
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6489,23 +6910,23 @@
               <a:spcPct val="35000"/>
             </a:spcAft>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR" sz="800" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2696278" y="5344106"/>
-        <a:ext cx="138441" cy="138441"/>
+        <a:off x="3772827" y="5826806"/>
+        <a:ext cx="23388" cy="23388"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{53EE5430-A405-0C45-8C3D-56B9B7B4C5EE}">
+    <dsp:sp modelId="{DFF22F0D-7EB3-DB46-B99E-239BB764C2DC}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3002706" y="6480759"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="3974439" y="5464599"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6565,12 +6986,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6582,25 +7003,25 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>FP3 : Agir sur l'IHM</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP31 : Analyser le mouvement de la pupille à l'aide de la distance utilisateur-IHM</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3020075" y="6498128"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="3988345" y="5478505"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{CF5C0BC9-1C55-6D44-9740-9A1957FD4485}">
+    <dsp:sp modelId="{9FA40A36-B6C2-5140-97C1-947018A2B70F}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm rot="19457599">
-          <a:off x="4133828" y="6599579"/>
-          <a:ext cx="584243" cy="14392"/>
+        <a:xfrm rot="2142401">
+          <a:off x="3550637" y="6105871"/>
+          <a:ext cx="467768" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6611,10 +7032,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="584243" y="7196"/>
+                <a:pt x="467768" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6667,19 +7088,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4411343" y="6592169"/>
-        <a:ext cx="29212" cy="29212"/>
+        <a:off x="3772827" y="6099812"/>
+        <a:ext cx="23388" cy="23388"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{8F0E1068-96D7-094C-A746-F91F87169C20}">
+    <dsp:sp modelId="{0963A656-C5DC-AB41-8DEE-D65A14EA566F}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4663157" y="6139774"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="3974439" y="6010613"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6739,12 +7160,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6756,25 +7177,25 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>FP31 : Effectuer l'action</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP32 : Déduire l'action à effectuer</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4680526" y="6157143"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="3988345" y="6024519"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{78144F12-25BE-F943-8DB8-4D280CF8337F}">
+    <dsp:sp modelId="{F2B8E9EC-9E8D-EF4F-8069-8CF8FD8833B2}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5849193" y="6429087"/>
-          <a:ext cx="474414" cy="14392"/>
+        <a:xfrm rot="4986103">
+          <a:off x="873862" y="5491605"/>
+          <a:ext cx="3162470" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6785,10 +7206,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="474414" y="7196"/>
+                <a:pt x="3162470" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -6797,7 +7218,7 @@
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
+              <a:shade val="60000"/>
               <a:hueOff val="0"/>
               <a:satOff val="0"/>
               <a:lumOff val="0"/>
@@ -6826,7 +7247,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+          <a:pPr lvl="0" algn="ctr" defTabSz="266700">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6837,23 +7258,23 @@
               <a:spcPct val="35000"/>
             </a:spcAft>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+          <a:endParaRPr lang="fr-FR" sz="600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6074540" y="6424422"/>
-        <a:ext cx="23720" cy="23720"/>
+        <a:off x="2376035" y="5418180"/>
+        <a:ext cx="158123" cy="158123"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{EC0EB3A7-6AD7-5242-97AF-E79A69522BAB}">
+    <dsp:sp modelId="{53EE5430-A405-0C45-8C3D-56B9B7B4C5EE}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6323607" y="6139774"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="2645015" y="6829633"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -6913,12 +7334,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6930,25 +7351,25 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>Système d'exploitation</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP4 : Agir sur l'IHM</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6340976" y="6157143"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="2658921" y="6843539"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{48799966-5966-574A-BC3A-266F4C6BAF17}">
+    <dsp:sp modelId="{CF5C0BC9-1C55-6D44-9740-9A1957FD4485}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
-        <a:xfrm rot="2142401">
-          <a:off x="4133828" y="6940565"/>
-          <a:ext cx="584243" cy="14392"/>
+        <a:xfrm rot="19457599">
+          <a:off x="3550637" y="6924891"/>
+          <a:ext cx="467768" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6959,10 +7380,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="584243" y="7196"/>
+                <a:pt x="467768" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -7015,19 +7436,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4411343" y="6933155"/>
-        <a:ext cx="29212" cy="29212"/>
+        <a:off x="3772827" y="6918832"/>
+        <a:ext cx="23388" cy="23388"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{8DA6C1C2-E0BE-DE44-8DDE-6C55EBB1BE40}">
+    <dsp:sp modelId="{8F0E1068-96D7-094C-A746-F91F87169C20}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4663157" y="6821744"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="3974439" y="6556626"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -7087,12 +7508,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7104,25 +7525,25 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
-            <a:t>FP31 : Rendre l'action visible sur l'interface</a:t>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP41 : Effectuer l'action</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4680526" y="6839113"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="3988345" y="6570532"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{8767306D-9113-BC4B-81AA-7FB530A91291}">
+    <dsp:sp modelId="{78144F12-25BE-F943-8DB8-4D280CF8337F}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5849193" y="7111057"/>
-          <a:ext cx="474414" cy="14392"/>
+          <a:off x="4924027" y="6788387"/>
+          <a:ext cx="379835" cy="11271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7133,10 +7554,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="7196"/>
+                <a:pt x="0" y="5635"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="474414" y="7196"/>
+                <a:pt x="379835" y="5635"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -7189,19 +7610,19 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6074540" y="7106393"/>
-        <a:ext cx="23720" cy="23720"/>
+        <a:off x="5104449" y="6784527"/>
+        <a:ext cx="18991" cy="18991"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{8B5EE93D-B5D5-D545-9E38-B095AB10F5BE}">
+    <dsp:sp modelId="{EC0EB3A7-6AD7-5242-97AF-E79A69522BAB}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="6323607" y="6821744"/>
-          <a:ext cx="1186036" cy="593018"/>
+          <a:off x="5303863" y="6556626"/>
+          <a:ext cx="949588" cy="474794"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -7261,12 +7682,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="5715" tIns="5715" rIns="5715" bIns="5715" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="400050">
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7278,14 +7699,362 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr lang="fr-FR" sz="900" b="0" i="0" u="none" kern="1200"/>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>Système d'exploitation</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="5317769" y="6570532"/>
+        <a:ext cx="921776" cy="446982"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{48799966-5966-574A-BC3A-266F4C6BAF17}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm rot="2142401">
+          <a:off x="3550637" y="7197897"/>
+          <a:ext cx="467768" cy="11271"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="5635"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="467768" y="5635"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3772827" y="7191839"/>
+        <a:ext cx="23388" cy="23388"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{8DA6C1C2-E0BE-DE44-8DDE-6C55EBB1BE40}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3974439" y="7102640"/>
+          <a:ext cx="949588" cy="474794"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
+            <a:t>FP42 : Rendre l'action visible sur l'interface</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3988345" y="7116546"/>
+        <a:ext cx="921776" cy="446982"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{8767306D-9113-BC4B-81AA-7FB530A91291}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4924027" y="7334401"/>
+          <a:ext cx="379835" cy="11271"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="5635"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="379835" y="5635"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="222250">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR" sz="500" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="5104449" y="7330541"/>
+        <a:ext cx="18991" cy="18991"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{8B5EE93D-B5D5-D545-9E38-B095AB10F5BE}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="5303863" y="7102640"/>
+          <a:ext cx="949588" cy="474794"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="4445" tIns="4445" rIns="4445" bIns="4445" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="311150">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="700" b="0" i="0" u="none" kern="1200"/>
             <a:t>Interface graphique</a:t>
           </a:r>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="6340976" y="6839113"/>
-        <a:ext cx="1151298" cy="558280"/>
+        <a:off x="5317769" y="7116546"/>
+        <a:ext cx="921776" cy="446982"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -9005,8 +9774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>